<commit_message>
Add opus base AoN results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2121" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32134D08-9AE7-4A80-B2BC-78A30C1B0EC0}"/>
+  <xr:revisionPtr revIDLastSave="2230" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2095AEE-ADB3-4653-8DE7-7B1712F66680}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
     <sheet name="opus_base Simple aWCE" sheetId="10" r:id="rId2"/>
-    <sheet name="opus_base Fine aWCE" sheetId="12" r:id="rId3"/>
-    <sheet name="opus_base AoN aWCE" sheetId="13" r:id="rId4"/>
+    <sheet name="opus_base AoN aWCE" sheetId="13" r:id="rId3"/>
+    <sheet name="opus_base Fine aWCE" sheetId="12" r:id="rId4"/>
     <sheet name="opus_base LSP Simple aWCE " sheetId="14" r:id="rId5"/>
-    <sheet name="opus_base LSP Fine aWCE " sheetId="15" r:id="rId6"/>
-    <sheet name="opus_base LSP AoN aWCE " sheetId="16" r:id="rId7"/>
+    <sheet name="opus_base LSP AoN aWCE " sheetId="16" r:id="rId6"/>
+    <sheet name="opus_base LSP Fine aWCE " sheetId="15" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -470,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -562,6 +562,66 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -571,24 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -619,39 +661,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -667,13 +676,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1005,13 +1008,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="52" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="52">
+      <c r="C2" s="36">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1033,9 +1036,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="54"/>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1055,9 +1058,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="54"/>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1077,9 +1080,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="54"/>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1099,9 +1102,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="54"/>
-      <c r="B6" s="58"/>
-      <c r="C6" s="58">
+      <c r="A6" s="38"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1123,9 +1126,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="54"/>
-      <c r="B7" s="58"/>
-      <c r="C7" s="58"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1145,9 +1148,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="54"/>
-      <c r="B8" s="58"/>
-      <c r="C8" s="58"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1167,9 +1170,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="54"/>
-      <c r="B9" s="58"/>
-      <c r="C9" s="58"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1189,9 +1192,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="58"/>
-      <c r="C10" s="58">
+      <c r="A10" s="38"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1213,9 +1216,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="54"/>
-      <c r="B11" s="58"/>
-      <c r="C11" s="58"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1235,9 +1238,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="54"/>
-      <c r="B12" s="58"/>
-      <c r="C12" s="58"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1257,9 +1260,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="54"/>
-      <c r="B13" s="58"/>
-      <c r="C13" s="58"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1279,9 +1282,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="54"/>
-      <c r="B14" s="58"/>
-      <c r="C14" s="58">
+      <c r="A14" s="38"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1303,9 +1306,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="54"/>
-      <c r="B15" s="58"/>
-      <c r="C15" s="58"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1325,9 +1328,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="54"/>
-      <c r="B16" s="58"/>
-      <c r="C16" s="58"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1347,9 +1350,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="54"/>
-      <c r="B17" s="58"/>
-      <c r="C17" s="58"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1369,11 +1372,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="54"/>
-      <c r="B18" s="50">
+      <c r="A18" s="38"/>
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="58"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1393,9 +1396,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
-      <c r="B19" s="51"/>
-      <c r="C19" s="58"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1415,9 +1418,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
-      <c r="B20" s="51"/>
-      <c r="C20" s="58"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1437,9 +1440,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="58"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1459,11 +1462,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
-      <c r="B22" s="58">
+      <c r="A22" s="38"/>
+      <c r="B22" s="44">
         <v>0.75</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1483,9 +1486,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
-      <c r="B23" s="58"/>
-      <c r="C23" s="58"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1504,9 +1507,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
-      <c r="B24" s="58"/>
-      <c r="C24" s="58"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1526,9 +1529,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
-      <c r="B25" s="58"/>
-      <c r="C25" s="58"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1548,11 +1551,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
-      <c r="B26" s="58">
+      <c r="A26" s="38"/>
+      <c r="B26" s="44">
         <v>0.5</v>
       </c>
-      <c r="C26" s="58"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1572,9 +1575,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
-      <c r="B27" s="58"/>
-      <c r="C27" s="58"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1597,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
-      <c r="B28" s="58"/>
-      <c r="C28" s="58"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1616,9 +1619,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
-      <c r="B29" s="58"/>
-      <c r="C29" s="58"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1638,11 +1641,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
-      <c r="B30" s="58">
+      <c r="A30" s="38"/>
+      <c r="B30" s="44">
         <v>0.25</v>
       </c>
-      <c r="C30" s="58"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1662,9 +1665,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
-      <c r="B31" s="58"/>
-      <c r="C31" s="58"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1684,9 +1687,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
-      <c r="B32" s="58"/>
-      <c r="C32" s="58"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1706,9 +1709,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="55"/>
-      <c r="B33" s="59"/>
-      <c r="C33" s="59"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1728,13 +1731,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="60">
+      <c r="B34" s="46">
         <v>0.1</v>
       </c>
-      <c r="C34" s="60">
+      <c r="C34" s="46">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1756,9 +1759,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="36"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="58"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1778,9 +1781,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="58"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1800,9 +1803,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="35"/>
-      <c r="B37" s="59"/>
-      <c r="C37" s="59"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1822,14 +1825,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="34" t="s">
+      <c r="A38" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="41"/>
-      <c r="D38" s="42"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1846,12 +1849,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="35"/>
-      <c r="B39" s="37" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="38"/>
-      <c r="D39" s="39"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1868,13 +1871,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="34" t="s">
+      <c r="A40" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="47" t="s">
+      <c r="B40" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="48"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1896,9 +1899,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="36"/>
-      <c r="B41" s="40"/>
-      <c r="C41" s="49"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1923,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="36"/>
-      <c r="B42" s="43" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="44"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1946,9 +1949,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="35"/>
-      <c r="B43" s="45"/>
-      <c r="C43" s="46"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1970,14 +1973,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="34" t="s">
+      <c r="A44" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="31" t="s">
+      <c r="B44" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="32"/>
-      <c r="D44" s="33"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1994,12 +1997,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="35"/>
-      <c r="B45" s="37" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="39"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2016,12 +2019,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="57" t="s">
+      <c r="A46" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="57"/>
-      <c r="C46" s="57"/>
-      <c r="D46" s="57"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2048,6 +2051,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2064,13 +2074,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2081,8 +2084,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C20E6-94C4-4B99-8775-24B7DED1396E}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2121,10 +2124,10 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="64">
         <v>4</v>
       </c>
       <c r="C2" s="25">
@@ -2147,8 +2150,8 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
@@ -2169,8 +2172,8 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="23">
         <v>1.75</v>
       </c>
@@ -2191,8 +2194,8 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="23">
         <v>2</v>
       </c>
@@ -2213,8 +2216,8 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="64">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67">
         <v>5</v>
       </c>
       <c r="C6" s="25">
@@ -2237,8 +2240,8 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="23">
         <v>1.5</v>
       </c>
@@ -2259,8 +2262,8 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="23">
         <v>1.75</v>
       </c>
@@ -2281,8 +2284,8 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="23">
         <v>2</v>
       </c>
@@ -2303,8 +2306,8 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="64">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67">
         <v>6</v>
       </c>
       <c r="C10" s="25">
@@ -2327,8 +2330,8 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="23">
         <v>1.5</v>
       </c>
@@ -2349,8 +2352,8 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
@@ -2371,8 +2374,8 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="23">
         <v>2</v>
       </c>
@@ -2393,8 +2396,8 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="64">
+      <c r="A14" s="65"/>
+      <c r="B14" s="67">
         <v>7</v>
       </c>
       <c r="C14" s="25">
@@ -2417,8 +2420,8 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
@@ -2439,8 +2442,8 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="23">
         <v>1.75</v>
       </c>
@@ -2461,8 +2464,8 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="23">
         <v>2</v>
       </c>
@@ -2483,10 +2486,10 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="68">
         <v>4</v>
       </c>
       <c r="C18" s="25">
@@ -2509,8 +2512,8 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
       </c>
@@ -2531,8 +2534,8 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
       </c>
@@ -2553,8 +2556,8 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
       </c>
@@ -2575,8 +2578,8 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="65">
+      <c r="A22" s="35"/>
+      <c r="B22" s="68">
         <v>5</v>
       </c>
       <c r="C22" s="25">
@@ -2599,8 +2602,8 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
       </c>
@@ -2620,8 +2623,8 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
       </c>
@@ -2642,8 +2645,8 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
       </c>
@@ -2664,8 +2667,8 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
-      <c r="B26" s="65">
+      <c r="A26" s="35"/>
+      <c r="B26" s="68">
         <v>6</v>
       </c>
       <c r="C26" s="25">
@@ -2688,8 +2691,8 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
@@ -2710,8 +2713,8 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
       </c>
@@ -2732,8 +2735,8 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
       </c>
@@ -2754,8 +2757,8 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="65">
+      <c r="A30" s="35"/>
+      <c r="B30" s="68">
         <v>7</v>
       </c>
       <c r="C30" s="25">
@@ -2778,8 +2781,8 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
       </c>
@@ -2800,8 +2803,8 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="65"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
       </c>
@@ -2822,8 +2825,8 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
       </c>
@@ -3014,6 +3017,727 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B44CA5E-D6A9-491D-9F24-D323A0E66CBD}">
+  <dimension ref="A1:I33"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.77734375" style="30" customWidth="1"/>
+    <col min="2" max="2" width="26.44140625" style="30" customWidth="1"/>
+    <col min="3" max="4" width="26.6640625" style="30" customWidth="1"/>
+    <col min="5" max="7" width="26.77734375" style="30" customWidth="1"/>
+    <col min="8" max="8" width="26.6640625" style="30" customWidth="1"/>
+    <col min="9" max="9" width="17.77734375" style="30" customWidth="1"/>
+    <col min="10" max="16384" width="8.88671875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="64" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="64">
+        <v>0.2</v>
+      </c>
+      <c r="C2" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D2" s="4">
+        <v>42.702100000000002</v>
+      </c>
+      <c r="E2" s="14">
+        <v>17217.2395</v>
+      </c>
+      <c r="F2" s="19">
+        <f t="shared" ref="F2:F18" si="0">E2/3600</f>
+        <v>4.782566527777778</v>
+      </c>
+      <c r="G2" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D3" s="6">
+        <v>42.737499999999997</v>
+      </c>
+      <c r="E3" s="15">
+        <v>19008.7209</v>
+      </c>
+      <c r="F3" s="19">
+        <f t="shared" si="0"/>
+        <v>5.28020025</v>
+      </c>
+      <c r="G3" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D4" s="6">
+        <v>42.5548</v>
+      </c>
+      <c r="E4" s="15">
+        <v>17271.606800000001</v>
+      </c>
+      <c r="F4" s="19">
+        <f t="shared" si="0"/>
+        <v>4.797668555555556</v>
+      </c>
+      <c r="G4" s="7">
+        <v>117.2388</v>
+      </c>
+      <c r="I4" s="69"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="23">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>42.728700000000003</v>
+      </c>
+      <c r="E5" s="15">
+        <v>20657.942500000001</v>
+      </c>
+      <c r="F5" s="19">
+        <f t="shared" si="0"/>
+        <v>5.7383173611111111</v>
+      </c>
+      <c r="G5" s="7">
+        <v>117.2388</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67">
+        <v>0.4</v>
+      </c>
+      <c r="C6" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D6" s="6">
+        <v>42.873399999999997</v>
+      </c>
+      <c r="E6" s="15">
+        <v>25416.178100000001</v>
+      </c>
+      <c r="F6" s="19">
+        <f t="shared" si="0"/>
+        <v>7.0600494722222225</v>
+      </c>
+      <c r="G6" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D7" s="6">
+        <v>42.848500000000001</v>
+      </c>
+      <c r="E7" s="15">
+        <v>23798.757699999998</v>
+      </c>
+      <c r="F7" s="19">
+        <f t="shared" si="0"/>
+        <v>6.6107660277777773</v>
+      </c>
+      <c r="G7" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D8" s="6">
+        <v>42.6203</v>
+      </c>
+      <c r="E8" s="15">
+        <v>16067.453799999999</v>
+      </c>
+      <c r="F8" s="19">
+        <f t="shared" si="0"/>
+        <v>4.4631816111111107</v>
+      </c>
+      <c r="G8" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="23">
+        <v>2</v>
+      </c>
+      <c r="D9" s="6">
+        <v>42.587299999999999</v>
+      </c>
+      <c r="E9" s="15">
+        <v>17407.544699999999</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>4.8354290833333327</v>
+      </c>
+      <c r="G9" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="C10" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D10" s="6">
+        <v>42.3277</v>
+      </c>
+      <c r="E10" s="15">
+        <v>15134.318600000001</v>
+      </c>
+      <c r="F10" s="19">
+        <f t="shared" si="0"/>
+        <v>4.2039773888888892</v>
+      </c>
+      <c r="G10" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D11" s="6">
+        <v>42.418700000000001</v>
+      </c>
+      <c r="E11" s="15">
+        <v>17504.587299999999</v>
+      </c>
+      <c r="F11" s="19">
+        <f t="shared" si="0"/>
+        <v>4.8623853611111105</v>
+      </c>
+      <c r="G11" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D12" s="6">
+        <v>41.464199999999998</v>
+      </c>
+      <c r="E12" s="15">
+        <v>8568.4732999999997</v>
+      </c>
+      <c r="F12" s="19">
+        <f t="shared" si="0"/>
+        <v>2.3801314722222222</v>
+      </c>
+      <c r="G12" s="7">
+        <v>27.621300000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="65"/>
+      <c r="B13" s="66"/>
+      <c r="C13" s="23">
+        <v>2</v>
+      </c>
+      <c r="D13" s="6">
+        <v>42.8294</v>
+      </c>
+      <c r="E13" s="15">
+        <v>23575.140299999999</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" si="0"/>
+        <v>6.5486500833333334</v>
+      </c>
+      <c r="G13" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="65"/>
+      <c r="B14" s="68">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D14" s="6">
+        <v>42.453299999999999</v>
+      </c>
+      <c r="E14" s="16">
+        <v>15651.1404</v>
+      </c>
+      <c r="F14" s="19">
+        <f t="shared" si="0"/>
+        <v>4.3475390000000003</v>
+      </c>
+      <c r="G14" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="65"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D15" s="6">
+        <v>42.844499999999996</v>
+      </c>
+      <c r="E15" s="15">
+        <v>16197.331099999999</v>
+      </c>
+      <c r="F15" s="19">
+        <f t="shared" si="0"/>
+        <v>4.4992586388888887</v>
+      </c>
+      <c r="G15" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="65"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D16" s="6">
+        <v>42.287599999999998</v>
+      </c>
+      <c r="E16" s="15">
+        <v>15399.1762</v>
+      </c>
+      <c r="F16" s="19">
+        <f t="shared" si="0"/>
+        <v>4.2775489444444448</v>
+      </c>
+      <c r="G16" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="66"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="23">
+        <v>2</v>
+      </c>
+      <c r="D17" s="6">
+        <v>42.500799999999998</v>
+      </c>
+      <c r="E17" s="16">
+        <v>16000.301600000001</v>
+      </c>
+      <c r="F17" s="19">
+        <f t="shared" si="0"/>
+        <v>4.444528222222222</v>
+      </c>
+      <c r="G17" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="65">
+        <v>0.2</v>
+      </c>
+      <c r="C18" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D18" s="6">
+        <v>42.648099999999999</v>
+      </c>
+      <c r="E18" s="16">
+        <v>17592.232599999999</v>
+      </c>
+      <c r="F18" s="19">
+        <f t="shared" si="0"/>
+        <v>4.8867312777777778</v>
+      </c>
+      <c r="G18" s="7">
+        <v>117.2388</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="35"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D19" s="6">
+        <v>42.956299999999999</v>
+      </c>
+      <c r="E19" s="16">
+        <v>25320.490600000001</v>
+      </c>
+      <c r="F19" s="19">
+        <f>E19/3600</f>
+        <v>7.0334696111111112</v>
+      </c>
+      <c r="G19" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="35"/>
+      <c r="B20" s="65"/>
+      <c r="C20" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D20" s="6">
+        <v>42.490900000000003</v>
+      </c>
+      <c r="E20" s="16">
+        <v>15511.254499999999</v>
+      </c>
+      <c r="F20" s="19">
+        <f t="shared" ref="F20:F33" si="1">E20/3600</f>
+        <v>4.3086818055555556</v>
+      </c>
+      <c r="G20" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="35"/>
+      <c r="B21" s="66"/>
+      <c r="C21" s="23">
+        <v>2</v>
+      </c>
+      <c r="D21" s="6">
+        <v>42.452800000000003</v>
+      </c>
+      <c r="E21" s="16">
+        <v>15414.6432</v>
+      </c>
+      <c r="F21" s="19">
+        <f t="shared" si="1"/>
+        <v>4.2818453333333331</v>
+      </c>
+      <c r="G21" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="35"/>
+      <c r="B22" s="67">
+        <v>0.4</v>
+      </c>
+      <c r="C22" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D22" s="6">
+        <v>42.461300000000001</v>
+      </c>
+      <c r="E22" s="16">
+        <v>14137.963900000001</v>
+      </c>
+      <c r="F22" s="19">
+        <f t="shared" si="1"/>
+        <v>3.9272121944444445</v>
+      </c>
+      <c r="G22" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="35"/>
+      <c r="B23" s="65"/>
+      <c r="C23" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D23" s="6">
+        <v>42.7879</v>
+      </c>
+      <c r="E23" s="16">
+        <v>25338.7857</v>
+      </c>
+      <c r="F23" s="19">
+        <f t="shared" si="1"/>
+        <v>7.0385515833333336</v>
+      </c>
+      <c r="G23" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="35"/>
+      <c r="B24" s="65"/>
+      <c r="C24" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D24" s="6">
+        <v>42.816600000000001</v>
+      </c>
+      <c r="E24" s="16">
+        <v>25830.7084</v>
+      </c>
+      <c r="F24" s="19">
+        <f t="shared" si="1"/>
+        <v>7.1751967777777779</v>
+      </c>
+      <c r="G24" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="35"/>
+      <c r="B25" s="66"/>
+      <c r="C25" s="23">
+        <v>2</v>
+      </c>
+      <c r="D25" s="6">
+        <v>42.893900000000002</v>
+      </c>
+      <c r="E25" s="16">
+        <v>22675.105200000002</v>
+      </c>
+      <c r="F25" s="19">
+        <f t="shared" si="1"/>
+        <v>6.2986403333333341</v>
+      </c>
+      <c r="G25" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="35"/>
+      <c r="B26" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="C26" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D26" s="6">
+        <v>42.756799999999998</v>
+      </c>
+      <c r="E26" s="16">
+        <v>17946.270400000001</v>
+      </c>
+      <c r="F26" s="19">
+        <f t="shared" si="1"/>
+        <v>4.9850751111111116</v>
+      </c>
+      <c r="G26" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="35"/>
+      <c r="B27" s="65"/>
+      <c r="C27" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D27" s="12">
+        <v>43.082599999999999</v>
+      </c>
+      <c r="E27" s="16">
+        <v>23625.376100000001</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="1"/>
+        <v>6.5626044722222225</v>
+      </c>
+      <c r="G27" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="35"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D28" s="6">
+        <v>42.710799999999999</v>
+      </c>
+      <c r="E28" s="16">
+        <v>16154.835499999999</v>
+      </c>
+      <c r="F28" s="19">
+        <f t="shared" si="1"/>
+        <v>4.4874543055555556</v>
+      </c>
+      <c r="G28" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="35"/>
+      <c r="B29" s="66"/>
+      <c r="C29" s="23">
+        <v>2</v>
+      </c>
+      <c r="D29" s="6">
+        <v>42.746400000000001</v>
+      </c>
+      <c r="E29" s="16">
+        <v>16132.570599999999</v>
+      </c>
+      <c r="F29" s="19">
+        <f t="shared" si="1"/>
+        <v>4.4812696111111112</v>
+      </c>
+      <c r="G29" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="35"/>
+      <c r="B30" s="67">
+        <v>0.8</v>
+      </c>
+      <c r="C30" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="D30" s="6">
+        <v>42.915700000000001</v>
+      </c>
+      <c r="E30" s="16">
+        <v>23288.329099999999</v>
+      </c>
+      <c r="F30" s="19">
+        <f t="shared" si="1"/>
+        <v>6.4689803055555553</v>
+      </c>
+      <c r="G30" s="7">
+        <v>137.96010000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="35"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="6">
+        <v>42.592100000000002</v>
+      </c>
+      <c r="E31" s="16">
+        <v>18890.779900000001</v>
+      </c>
+      <c r="F31" s="19">
+        <f t="shared" si="1"/>
+        <v>5.2474388611111111</v>
+      </c>
+      <c r="G31" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="35"/>
+      <c r="B32" s="65"/>
+      <c r="C32" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="D32" s="6">
+        <v>42.393799999999999</v>
+      </c>
+      <c r="E32" s="16">
+        <v>14328.2937</v>
+      </c>
+      <c r="F32" s="19">
+        <f t="shared" si="1"/>
+        <v>3.9800815833333334</v>
+      </c>
+      <c r="G32" s="7">
+        <v>103.4885</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="36"/>
+      <c r="B33" s="66"/>
+      <c r="C33" s="23">
+        <v>2</v>
+      </c>
+      <c r="D33" s="6">
+        <v>42.602400000000003</v>
+      </c>
+      <c r="E33" s="16">
+        <v>15981.097599999999</v>
+      </c>
+      <c r="F33" s="19">
+        <f t="shared" si="1"/>
+        <v>4.4391937777777777</v>
+      </c>
+      <c r="G33" s="7">
+        <v>82.794399999999996</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4007DDC-E746-4472-AC8B-DF55C0CDCC5B}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -3056,10 +3780,10 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="61">
+      <c r="B2" s="64">
         <v>0</v>
       </c>
       <c r="C2" s="25">
@@ -3071,8 +3795,8 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
+      <c r="A3" s="65"/>
+      <c r="B3" s="65"/>
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
@@ -3082,8 +3806,8 @@
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
+      <c r="A4" s="65"/>
+      <c r="B4" s="65"/>
       <c r="C4" s="23">
         <v>1.75</v>
       </c>
@@ -3093,8 +3817,8 @@
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
+      <c r="A5" s="65"/>
+      <c r="B5" s="66"/>
       <c r="C5" s="23">
         <v>2</v>
       </c>
@@ -3104,8 +3828,8 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="64">
+      <c r="A6" s="65"/>
+      <c r="B6" s="67">
         <v>1</v>
       </c>
       <c r="C6" s="25">
@@ -3117,8 +3841,8 @@
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="65"/>
       <c r="C7" s="23">
         <v>1.5</v>
       </c>
@@ -3128,8 +3852,8 @@
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="23">
         <v>1.75</v>
       </c>
@@ -3139,8 +3863,8 @@
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="23">
         <v>2</v>
       </c>
@@ -3150,8 +3874,8 @@
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="64">
+      <c r="A10" s="65"/>
+      <c r="B10" s="67">
         <v>2</v>
       </c>
       <c r="C10" s="25">
@@ -3163,8 +3887,8 @@
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
+      <c r="A11" s="65"/>
+      <c r="B11" s="65"/>
       <c r="C11" s="23">
         <v>1.5</v>
       </c>
@@ -3174,8 +3898,8 @@
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
+      <c r="A12" s="65"/>
+      <c r="B12" s="65"/>
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
@@ -3185,8 +3909,8 @@
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
+      <c r="A13" s="65"/>
+      <c r="B13" s="66"/>
       <c r="C13" s="23">
         <v>2</v>
       </c>
@@ -3196,8 +3920,8 @@
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="64">
+      <c r="A14" s="65"/>
+      <c r="B14" s="67">
         <v>3</v>
       </c>
       <c r="C14" s="25">
@@ -3209,8 +3933,8 @@
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="62"/>
+      <c r="A15" s="65"/>
+      <c r="B15" s="65"/>
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
@@ -3220,8 +3944,8 @@
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
-      <c r="B16" s="62"/>
+      <c r="A16" s="65"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="23">
         <v>1.75</v>
       </c>
@@ -3231,8 +3955,8 @@
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
+      <c r="A17" s="66"/>
+      <c r="B17" s="66"/>
       <c r="C17" s="23">
         <v>2</v>
       </c>
@@ -3242,10 +3966,10 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="65">
+      <c r="B18" s="68">
         <v>0</v>
       </c>
       <c r="C18" s="25">
@@ -3257,8 +3981,8 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="65"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
       </c>
@@ -3268,8 +3992,8 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="65"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
       </c>
@@ -3279,8 +4003,8 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="65"/>
+      <c r="A21" s="35"/>
+      <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
       </c>
@@ -3290,8 +4014,8 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="65">
+      <c r="A22" s="35"/>
+      <c r="B22" s="68">
         <v>1</v>
       </c>
       <c r="C22" s="25">
@@ -3303,8 +4027,8 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="65"/>
+      <c r="A23" s="35"/>
+      <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
       </c>
@@ -3314,8 +4038,8 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="65"/>
+      <c r="A24" s="35"/>
+      <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
       </c>
@@ -3325,8 +4049,8 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="65"/>
+      <c r="A25" s="35"/>
+      <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
       </c>
@@ -3336,8 +4060,8 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
-      <c r="B26" s="65">
+      <c r="A26" s="35"/>
+      <c r="B26" s="68">
         <v>2</v>
       </c>
       <c r="C26" s="25">
@@ -3349,8 +4073,8 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="65"/>
+      <c r="A27" s="35"/>
+      <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
@@ -3360,8 +4084,8 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="65"/>
+      <c r="A28" s="35"/>
+      <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
       </c>
@@ -3371,8 +4095,8 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="65"/>
+      <c r="A29" s="35"/>
+      <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
       </c>
@@ -3382,8 +4106,8 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="65">
+      <c r="A30" s="35"/>
+      <c r="B30" s="68">
         <v>3</v>
       </c>
       <c r="C30" s="25">
@@ -3395,8 +4119,8 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="65"/>
+      <c r="A31" s="35"/>
+      <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
       </c>
@@ -3406,8 +4130,8 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="65"/>
+      <c r="A32" s="35"/>
+      <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
       </c>
@@ -3417,8 +4141,8 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="65"/>
+      <c r="A33" s="36"/>
+      <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
       </c>
@@ -3431,448 +4155,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B44CA5E-D6A9-491D-9F24-D323A0E66CBD}">
-  <dimension ref="A1:G33"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="21.77734375" style="30" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="30" customWidth="1"/>
-    <col min="3" max="4" width="26.6640625" style="30" customWidth="1"/>
-    <col min="5" max="7" width="26.77734375" style="30" customWidth="1"/>
-    <col min="8" max="8" width="26.6640625" style="30" customWidth="1"/>
-    <col min="9" max="9" width="17.77734375" style="30" customWidth="1"/>
-    <col min="10" max="16384" width="8.88671875" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="61" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="C2" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="62"/>
-      <c r="C3" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="62"/>
-      <c r="C4" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="23">
-        <v>2</v>
-      </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="62"/>
-      <c r="B6" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="C6" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="62"/>
-      <c r="C7" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="62"/>
-      <c r="C8" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="62"/>
-      <c r="B9" s="63"/>
-      <c r="C9" s="23">
-        <v>2</v>
-      </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="62"/>
-      <c r="B10" s="64">
-        <v>0.6</v>
-      </c>
-      <c r="C10" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="62"/>
-      <c r="C11" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="62"/>
-      <c r="C12" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="62"/>
-      <c r="B13" s="63"/>
-      <c r="C13" s="23">
-        <v>2</v>
-      </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="62"/>
-      <c r="B14" s="65">
-        <v>0.8</v>
-      </c>
-      <c r="C14" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="16"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
-      <c r="B15" s="65"/>
-      <c r="C15" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
-      <c r="B17" s="65"/>
-      <c r="C17" s="23">
-        <v>2</v>
-      </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="16"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="7"/>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="50" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="62">
-        <v>0.2</v>
-      </c>
-      <c r="C18" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="16"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="7"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="51"/>
-      <c r="B19" s="62"/>
-      <c r="C19" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="7"/>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="51"/>
-      <c r="B20" s="62"/>
-      <c r="C20" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="16"/>
-      <c r="F20" s="19"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="51"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="23">
-        <v>2</v>
-      </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="51"/>
-      <c r="B22" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="C22" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="16"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="51"/>
-      <c r="B23" s="62"/>
-      <c r="C23" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="16"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="51"/>
-      <c r="B24" s="62"/>
-      <c r="C24" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="51"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="23">
-        <v>2</v>
-      </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="16"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="51"/>
-      <c r="B26" s="64">
-        <v>0.6</v>
-      </c>
-      <c r="C26" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="16"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="7"/>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="51"/>
-      <c r="B27" s="62"/>
-      <c r="C27" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="16"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="7"/>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="51"/>
-      <c r="B28" s="62"/>
-      <c r="C28" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="16"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="7"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="51"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="23">
-        <v>2</v>
-      </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="7"/>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="51"/>
-      <c r="B30" s="64">
-        <v>0.8</v>
-      </c>
-      <c r="C30" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="51"/>
-      <c r="B31" s="62"/>
-      <c r="C31" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="16"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="51"/>
-      <c r="B32" s="62"/>
-      <c r="C32" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="16"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="7"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="52"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="23">
-        <v>2</v>
-      </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="16"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="7"/>
-    </row>
-  </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3919,7 +4211,7 @@
       <c r="H1" s="10"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="61">
+      <c r="A2" s="64">
         <v>4</v>
       </c>
       <c r="B2" s="25">
@@ -3933,7 +4225,7 @@
       <c r="H2" s="10"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="23">
         <v>1.5</v>
       </c>
@@ -3945,7 +4237,7 @@
       <c r="H3" s="10"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="23">
         <v>1.75</v>
       </c>
@@ -3957,7 +4249,7 @@
       <c r="H4" s="10"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="23">
         <v>2</v>
       </c>
@@ -3969,7 +4261,7 @@
       <c r="H5" s="10"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="64">
+      <c r="A6" s="67">
         <v>5</v>
       </c>
       <c r="B6" s="25">
@@ -3983,7 +4275,7 @@
       <c r="H6" s="10"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="23">
         <v>1.5</v>
       </c>
@@ -3995,7 +4287,7 @@
       <c r="H7" s="10"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="23">
         <v>1.75</v>
       </c>
@@ -4007,7 +4299,7 @@
       <c r="H8" s="10"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="63"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="23">
         <v>2</v>
       </c>
@@ -4019,7 +4311,7 @@
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="64">
+      <c r="A10" s="67">
         <v>6</v>
       </c>
       <c r="B10" s="25">
@@ -4033,7 +4325,7 @@
       <c r="H10" s="10"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="23">
         <v>1.5</v>
       </c>
@@ -4045,7 +4337,7 @@
       <c r="H11" s="10"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="23">
         <v>1.75</v>
       </c>
@@ -4057,7 +4349,7 @@
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
       </c>
@@ -4069,7 +4361,7 @@
       <c r="H13" s="10"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="64">
+      <c r="A14" s="67">
         <v>7</v>
       </c>
       <c r="B14" s="25">
@@ -4083,7 +4375,7 @@
       <c r="H14" s="10"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="23">
         <v>1.5</v>
       </c>
@@ -4095,7 +4387,7 @@
       <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="23">
         <v>1.75</v>
       </c>
@@ -4107,7 +4399,7 @@
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="23">
         <v>2</v>
       </c>
@@ -4119,191 +4411,191 @@
       <c r="H17" s="10"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
       <c r="G18" s="28"/>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
       <c r="G19" s="28"/>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
       <c r="G20" s="28"/>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
       <c r="G21" s="28"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
       <c r="G22" s="28"/>
       <c r="H22" s="10"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
       <c r="G23" s="28"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
       <c r="G24" s="28"/>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
       <c r="G25" s="28"/>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
       <c r="G26" s="28"/>
       <c r="H26" s="10"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
       <c r="G27" s="28"/>
       <c r="H27" s="10"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
       <c r="G28" s="28"/>
       <c r="H28" s="10"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
       <c r="G29" s="28"/>
       <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="67"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
       <c r="G30" s="28"/>
       <c r="H30" s="10"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
       <c r="G31" s="28"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
       <c r="G32" s="28"/>
       <c r="H32" s="10"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
       <c r="G33" s="28"/>
       <c r="H33" s="10"/>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
       <c r="G34" s="28"/>
       <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" s="67"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
       <c r="G35" s="28"/>
       <c r="H35" s="10"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
       <c r="G36" s="28"/>
       <c r="H36" s="10"/>
     </row>
@@ -4429,6 +4721,376 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71968B89-5396-4DBB-9374-8D1D5CD3665B}">
+  <dimension ref="A1:F36"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I32" sqref="I32"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" style="30" customWidth="1"/>
+    <col min="2" max="3" width="26.6640625" style="30" customWidth="1"/>
+    <col min="4" max="6" width="26.77734375" style="30" customWidth="1"/>
+    <col min="7" max="7" width="26.6640625" style="30" customWidth="1"/>
+    <col min="8" max="8" width="17.77734375" style="30" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="64">
+        <v>0.2</v>
+      </c>
+      <c r="B2" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="65"/>
+      <c r="B3" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="65"/>
+      <c r="B4" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="66"/>
+      <c r="B5" s="23">
+        <v>2</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="67">
+        <v>0.4</v>
+      </c>
+      <c r="B6" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="65"/>
+      <c r="B7" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="6"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="65"/>
+      <c r="B8" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="66"/>
+      <c r="B9" s="23">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="67">
+        <v>0.6</v>
+      </c>
+      <c r="B10" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="C10" s="6"/>
+      <c r="D10" s="15"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="65"/>
+      <c r="B11" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="65"/>
+      <c r="B12" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="66"/>
+      <c r="B13" s="23">
+        <v>2</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="15"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="68">
+        <v>0.8</v>
+      </c>
+      <c r="B14" s="25">
+        <v>1.25</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="16"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="68"/>
+      <c r="B15" s="23">
+        <v>1.5</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="15"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="68"/>
+      <c r="B16" s="23">
+        <v>1.75</v>
+      </c>
+      <c r="C16" s="6"/>
+      <c r="D16" s="15"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="68"/>
+      <c r="B17" s="23">
+        <v>2</v>
+      </c>
+      <c r="C17" s="6"/>
+      <c r="D17" s="16"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="32"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="32"/>
+      <c r="B35" s="32"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="32"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="32"/>
+      <c r="B36" s="32"/>
+      <c r="C36" s="32"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="32"/>
+      <c r="F36" s="32"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="A10:A13"/>
+    <mergeCell ref="A14:A17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEC7E3C-257D-4C00-940F-B3A10CBB9AD7}">
   <dimension ref="A1:G47"/>
   <sheetViews>
@@ -4467,7 +5129,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="61">
+      <c r="A2" s="64">
         <v>0</v>
       </c>
       <c r="B2" s="25">
@@ -4479,7 +5141,7 @@
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
+      <c r="A3" s="65"/>
       <c r="B3" s="23">
         <v>1.5</v>
       </c>
@@ -4489,7 +5151,7 @@
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
+      <c r="A4" s="65"/>
       <c r="B4" s="23">
         <v>1.75</v>
       </c>
@@ -4499,7 +5161,7 @@
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
+      <c r="A5" s="66"/>
       <c r="B5" s="23">
         <v>2</v>
       </c>
@@ -4509,7 +5171,7 @@
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="64">
+      <c r="A6" s="67">
         <v>1</v>
       </c>
       <c r="B6" s="25">
@@ -4521,7 +5183,7 @@
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
+      <c r="A7" s="65"/>
       <c r="B7" s="23">
         <v>1.5</v>
       </c>
@@ -4531,7 +5193,7 @@
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
+      <c r="A8" s="65"/>
       <c r="B8" s="23">
         <v>1.75</v>
       </c>
@@ -4541,7 +5203,7 @@
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="63"/>
+      <c r="A9" s="66"/>
       <c r="B9" s="23">
         <v>2</v>
       </c>
@@ -4551,7 +5213,7 @@
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="64">
+      <c r="A10" s="67">
         <v>2</v>
       </c>
       <c r="B10" s="25">
@@ -4563,7 +5225,7 @@
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
+      <c r="A11" s="65"/>
       <c r="B11" s="23">
         <v>1.5</v>
       </c>
@@ -4573,7 +5235,7 @@
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
+      <c r="A12" s="65"/>
       <c r="B12" s="23">
         <v>1.75</v>
       </c>
@@ -4583,7 +5245,7 @@
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
+      <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
       </c>
@@ -4593,7 +5255,7 @@
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="64">
+      <c r="A14" s="67">
         <v>3</v>
       </c>
       <c r="B14" s="25">
@@ -4605,7 +5267,7 @@
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="62"/>
+      <c r="A15" s="65"/>
       <c r="B15" s="23">
         <v>1.5</v>
       </c>
@@ -4615,7 +5277,7 @@
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="62"/>
+      <c r="A16" s="65"/>
       <c r="B16" s="23">
         <v>1.75</v>
       </c>
@@ -4625,7 +5287,7 @@
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="63"/>
+      <c r="A17" s="66"/>
       <c r="B17" s="23">
         <v>2</v>
       </c>
@@ -4635,157 +5297,157 @@
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="68"/>
-      <c r="B18" s="67"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="32"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="68"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="68"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="32"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="68"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+      <c r="F21" s="32"/>
+      <c r="G21" s="32"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="32"/>
+      <c r="F22" s="32"/>
+      <c r="G22" s="32"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="32"/>
+      <c r="F23" s="32"/>
+      <c r="G23" s="32"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
+      <c r="A25" s="32"/>
+      <c r="B25" s="32"/>
+      <c r="C25" s="32"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="32"/>
+      <c r="G25" s="32"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
+      <c r="A26" s="32"/>
+      <c r="B26" s="32"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="32"/>
+      <c r="F26" s="32"/>
+      <c r="G26" s="32"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-      <c r="G27" s="67"/>
+      <c r="A27" s="32"/>
+      <c r="B27" s="32"/>
+      <c r="C27" s="32"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="32"/>
+      <c r="F27" s="32"/>
+      <c r="G27" s="32"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-      <c r="G28" s="67"/>
+      <c r="A28" s="32"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="32"/>
+      <c r="F28" s="32"/>
+      <c r="G28" s="32"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="32"/>
+      <c r="F29" s="32"/>
+      <c r="G29" s="32"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="67"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
+      <c r="A30" s="32"/>
+      <c r="B30" s="32"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="32"/>
+      <c r="F30" s="32"/>
+      <c r="G30" s="32"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
+      <c r="A31" s="32"/>
+      <c r="B31" s="32"/>
+      <c r="C31" s="32"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="32"/>
+      <c r="G31" s="32"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-      <c r="G32" s="67"/>
+      <c r="A32" s="32"/>
+      <c r="B32" s="32"/>
+      <c r="C32" s="32"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="32"/>
+      <c r="F32" s="32"/>
+      <c r="G32" s="32"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-      <c r="G33" s="67"/>
+      <c r="A33" s="32"/>
+      <c r="B33" s="32"/>
+      <c r="C33" s="32"/>
+      <c r="D33" s="32"/>
+      <c r="E33" s="32"/>
+      <c r="F33" s="32"/>
+      <c r="G33" s="32"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
+      <c r="A34" s="32"/>
+      <c r="B34" s="32"/>
+      <c r="C34" s="32"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="32"/>
+      <c r="G34" s="32"/>
     </row>
     <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4801,382 +5463,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71968B89-5396-4DBB-9374-8D1D5CD3665B}">
-  <dimension ref="A1:F36"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="26.44140625" style="30" customWidth="1"/>
-    <col min="2" max="3" width="26.6640625" style="30" customWidth="1"/>
-    <col min="4" max="6" width="26.77734375" style="30" customWidth="1"/>
-    <col min="7" max="7" width="26.6640625" style="30" customWidth="1"/>
-    <col min="8" max="8" width="17.77734375" style="30" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="30"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="61">
-        <v>0.2</v>
-      </c>
-      <c r="B2" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="62"/>
-      <c r="B3" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="7"/>
-      <c r="F3" s="7"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="62"/>
-      <c r="B4" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="63"/>
-      <c r="B5" s="23">
-        <v>2</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="64">
-        <v>0.4</v>
-      </c>
-      <c r="B6" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62"/>
-      <c r="B7" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="62"/>
-      <c r="B8" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="63"/>
-      <c r="B9" s="23">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="64">
-        <v>0.6</v>
-      </c>
-      <c r="B10" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="62"/>
-      <c r="B11" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="62"/>
-      <c r="B12" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="63"/>
-      <c r="B13" s="23">
-        <v>2</v>
-      </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="65">
-        <v>0.8</v>
-      </c>
-      <c r="B14" s="25">
-        <v>1.25</v>
-      </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
-      <c r="B15" s="23">
-        <v>1.5</v>
-      </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="65"/>
-      <c r="B16" s="23">
-        <v>1.75</v>
-      </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
-      <c r="B17" s="23">
-        <v>2</v>
-      </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="66"/>
-      <c r="B18" s="66"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="66"/>
-      <c r="E18" s="66"/>
-      <c r="F18" s="66"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="67"/>
-      <c r="B19" s="67"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="67"/>
-      <c r="B21" s="67"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="67"/>
-      <c r="B22" s="67"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="67"/>
-      <c r="B23" s="67"/>
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="67"/>
-      <c r="B24" s="67"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="67"/>
-      <c r="B25" s="67"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="67"/>
-      <c r="B26" s="67"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="67"/>
-      <c r="B27" s="67"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="67"/>
-      <c r="E27" s="67"/>
-      <c r="F27" s="67"/>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="67"/>
-      <c r="B28" s="67"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="67"/>
-      <c r="E28" s="67"/>
-      <c r="F28" s="67"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="67"/>
-      <c r="B29" s="67"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="67"/>
-      <c r="E29" s="67"/>
-      <c r="F29" s="67"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="67"/>
-      <c r="B30" s="67"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="67"/>
-      <c r="E30" s="67"/>
-      <c r="F30" s="67"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="67"/>
-      <c r="B31" s="67"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="67"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="67"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="67"/>
-      <c r="B32" s="67"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="67"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="67"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="67"/>
-      <c r="B33" s="67"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="67"/>
-      <c r="E33" s="67"/>
-      <c r="F33" s="67"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="67"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="67"/>
-      <c r="B35" s="67"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="67"/>
-      <c r="F35" s="67"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="67"/>
-      <c r="B36" s="67"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="67"/>
-      <c r="E36" s="67"/>
-      <c r="F36" s="67"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A2:A5"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="A10:A13"/>
-    <mergeCell ref="A14:A17"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5409,27 +5702,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5454,9 +5737,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Redo hyperparameter search due to bugfix
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2230" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A2095AEE-ADB3-4653-8DE7-7B1712F66680}"/>
+  <xr:revisionPtr revIDLastSave="2338" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD1CA7A-BA30-4836-AF26-1F7B55760102}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
   <si>
     <t>Weight</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Weighted Proportion</t>
+  </si>
+  <si>
+    <t>RERUN</t>
   </si>
 </sst>
 </file>
@@ -470,7 +473,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -675,9 +678,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -966,7 +966,7 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
@@ -2085,7 +2085,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2134,17 +2134,17 @@
         <v>1.25</v>
       </c>
       <c r="D2" s="4">
-        <v>42.159300000000002</v>
+        <v>42.384999999999998</v>
       </c>
       <c r="E2" s="14">
-        <v>11410.3644</v>
+        <v>15226.288</v>
       </c>
       <c r="F2" s="5">
         <f>E2/3600</f>
-        <v>3.1695456666666666</v>
-      </c>
-      <c r="G2" s="5">
-        <v>75.895300000000006</v>
+        <v>4.2295244444444444</v>
+      </c>
+      <c r="G2" s="7">
+        <v>103.4885</v>
       </c>
       <c r="H2" s="28"/>
       <c r="I2" s="10"/>
@@ -2156,17 +2156,17 @@
         <v>1.5</v>
       </c>
       <c r="D3" s="6">
-        <v>42.777099999999997</v>
+        <v>42.421500000000002</v>
       </c>
       <c r="E3" s="15">
-        <v>17739.649000000001</v>
+        <v>21051.063200000001</v>
       </c>
       <c r="F3" s="5">
         <f>E3/3600</f>
-        <v>4.9276802777777782</v>
-      </c>
-      <c r="G3" s="7">
-        <v>82.794399999999996</v>
+        <v>5.8475175555555561</v>
+      </c>
+      <c r="G3" s="5">
+        <v>117.2388</v>
       </c>
       <c r="H3" s="28"/>
       <c r="I3" s="10"/>
@@ -2178,14 +2178,14 @@
         <v>1.75</v>
       </c>
       <c r="D4" s="6">
-        <v>41.983800000000002</v>
+        <v>41.7776</v>
       </c>
       <c r="E4" s="15">
-        <v>11161.4789</v>
+        <v>10650.197399999999</v>
       </c>
       <c r="F4" s="5">
         <f t="shared" ref="F4:F33" si="0">E4/3600</f>
-        <v>3.1004108055555557</v>
+        <v>2.9583881666666665</v>
       </c>
       <c r="G4" s="7">
         <v>41.391100000000002</v>
@@ -2200,17 +2200,17 @@
         <v>2</v>
       </c>
       <c r="D5" s="6">
-        <v>42.598599999999998</v>
+        <v>42.323700000000002</v>
       </c>
       <c r="E5" s="15">
-        <v>17996.982100000001</v>
+        <v>16833.3815</v>
       </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>4.999161694444445</v>
+        <v>4.6759393055555556</v>
       </c>
       <c r="G5" s="7">
-        <v>82.794399999999996</v>
+        <v>103.4885</v>
       </c>
       <c r="H5" s="28"/>
       <c r="I5" s="10"/>
@@ -2224,17 +2224,17 @@
         <v>1.25</v>
       </c>
       <c r="D6" s="6">
-        <v>42.009300000000003</v>
+        <v>42.469499999999996</v>
       </c>
       <c r="E6" s="15">
-        <v>12283.3434</v>
+        <v>15109.545099999999</v>
       </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>3.412039833333333</v>
+        <v>4.1970958611111113</v>
       </c>
       <c r="G6" s="7">
-        <v>82.794399999999996</v>
+        <v>103.4885</v>
       </c>
       <c r="H6" s="28"/>
       <c r="I6" s="10"/>
@@ -2246,14 +2246,14 @@
         <v>1.5</v>
       </c>
       <c r="D7" s="6">
-        <v>42.687399999999997</v>
+        <v>42.596800000000002</v>
       </c>
       <c r="E7" s="15">
-        <v>26355.5609</v>
+        <v>20139.2827</v>
       </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>7.3209891388888888</v>
+        <v>5.5942451944444445</v>
       </c>
       <c r="G7" s="7">
         <v>137.96010000000001</v>
@@ -2268,17 +2268,17 @@
         <v>1.75</v>
       </c>
       <c r="D8" s="6">
-        <v>42.670200000000001</v>
+        <v>41.914999999999999</v>
       </c>
       <c r="E8" s="15">
-        <v>17906.271499999999</v>
+        <v>11228.163500000001</v>
       </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>4.9739643055555556</v>
+        <v>3.1189343055555558</v>
       </c>
       <c r="G8" s="7">
-        <v>82.794399999999996</v>
+        <v>41.391100000000002</v>
       </c>
       <c r="H8" s="28"/>
       <c r="I8" s="10"/>
@@ -2290,14 +2290,14 @@
         <v>2</v>
       </c>
       <c r="D9" s="6">
-        <v>42.621000000000002</v>
+        <v>42.5366</v>
       </c>
       <c r="E9" s="15">
-        <v>25974.524799999999</v>
+        <v>20476.152300000002</v>
       </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>7.2151457777777779</v>
+        <v>5.6878200833333334</v>
       </c>
       <c r="G9" s="7">
         <v>137.96010000000001</v>
@@ -2314,17 +2314,17 @@
         <v>1.25</v>
       </c>
       <c r="D10" s="6">
-        <v>42.688000000000002</v>
+        <v>42.490099999999998</v>
       </c>
       <c r="E10" s="15">
-        <v>25070.5285</v>
+        <v>18328.035199999998</v>
       </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>6.9640356944444441</v>
-      </c>
-      <c r="G10" s="7">
-        <v>137.96010000000001</v>
+        <v>5.0911208888888888</v>
+      </c>
+      <c r="G10" s="5">
+        <v>117.2388</v>
       </c>
       <c r="H10" s="28"/>
       <c r="I10" s="10"/>
@@ -2336,14 +2336,14 @@
         <v>1.5</v>
       </c>
       <c r="D11" s="6">
-        <v>42.724899999999998</v>
+        <v>42.532499999999999</v>
       </c>
       <c r="E11" s="15">
-        <v>17261.7817</v>
+        <v>17255.9264</v>
       </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>4.7949393611111111</v>
+        <v>4.793312888888889</v>
       </c>
       <c r="G11" s="7">
         <v>82.794399999999996</v>
@@ -2357,20 +2357,16 @@
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
-      <c r="D12" s="6">
-        <v>42.436999999999998</v>
-      </c>
-      <c r="E12" s="15">
-        <v>18551.671399999999</v>
-      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>5.1532420555555554</v>
-      </c>
-      <c r="G12" s="5">
-        <v>117.2388</v>
-      </c>
-      <c r="H12" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2379,20 +2375,16 @@
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
-        <v>42.379300000000001</v>
-      </c>
-      <c r="E13" s="15">
-        <v>15339.9956</v>
-      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>4.261109888888889</v>
-      </c>
-      <c r="G13" s="7">
-        <v>103.4885</v>
-      </c>
-      <c r="H13" s="28"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2404,17 +2396,17 @@
         <v>1.25</v>
       </c>
       <c r="D14" s="6">
-        <v>42.7744</v>
+        <v>42.496899999999997</v>
       </c>
       <c r="E14" s="16">
-        <v>23624.459900000002</v>
+        <v>15313.7019</v>
       </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>6.5623499722222229</v>
+        <v>4.2538060833333331</v>
       </c>
       <c r="G14" s="7">
-        <v>137.96010000000001</v>
+        <v>69.000799999999998</v>
       </c>
       <c r="H14" s="28"/>
       <c r="I14" s="10"/>
@@ -2426,14 +2418,14 @@
         <v>1.5</v>
       </c>
       <c r="D15" s="6">
-        <v>42.704300000000003</v>
+        <v>42.741199999999999</v>
       </c>
       <c r="E15" s="15">
-        <v>17429.029699999999</v>
+        <v>17547.565299999998</v>
       </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>4.8413971388888886</v>
+        <v>4.8743236944444437</v>
       </c>
       <c r="G15" s="7">
         <v>82.794399999999996</v>
@@ -2448,17 +2440,17 @@
         <v>1.75</v>
       </c>
       <c r="D16" s="6">
-        <v>42.619399999999999</v>
+        <v>42.201700000000002</v>
       </c>
       <c r="E16" s="15">
-        <v>17118.860499999999</v>
+        <v>11294.0255</v>
       </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>4.7552390277777778</v>
+        <v>3.1372293055555556</v>
       </c>
       <c r="G16" s="7">
-        <v>82.794399999999996</v>
+        <v>75.895300000000006</v>
       </c>
       <c r="H16" s="28"/>
       <c r="I16" s="10"/>
@@ -2470,17 +2462,17 @@
         <v>2</v>
       </c>
       <c r="D17" s="6">
-        <v>42.021999999999998</v>
+        <v>42.299100000000003</v>
       </c>
       <c r="E17" s="16">
-        <v>11100.509599999999</v>
+        <v>15304.096299999999</v>
       </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>3.0834748888888885</v>
+        <v>4.2511378611111112</v>
       </c>
       <c r="G17" s="7">
-        <v>69.000799999999998</v>
+        <v>103.4885</v>
       </c>
       <c r="H17" s="28"/>
       <c r="I17" s="10"/>
@@ -2499,11 +2491,11 @@
         <v>42.597999999999999</v>
       </c>
       <c r="E18" s="14">
-        <v>17111.858800000002</v>
+        <v>17783.9172</v>
       </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>4.7532941111111118</v>
+        <v>4.9399769999999998</v>
       </c>
       <c r="G18" s="5">
         <v>117.2388</v>
@@ -2521,11 +2513,11 @@
         <v>42.517899999999997</v>
       </c>
       <c r="E19" s="15">
-        <v>15757.041499999999</v>
+        <v>15131.3624</v>
       </c>
       <c r="F19" s="5">
         <f>E19/3600</f>
-        <v>4.3769559722222224</v>
+        <v>4.2031562222222218</v>
       </c>
       <c r="G19" s="7">
         <v>82.794399999999996</v>
@@ -2543,11 +2535,11 @@
         <v>41.6218</v>
       </c>
       <c r="E20" s="15">
-        <v>8477.8197</v>
+        <v>8340.6447000000007</v>
       </c>
       <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>2.3549499166666665</v>
+        <v>2.3168457500000001</v>
       </c>
       <c r="G20" s="7">
         <v>55.2</v>
@@ -2565,11 +2557,11 @@
         <v>42.6858</v>
       </c>
       <c r="E21" s="15">
-        <v>17872.459200000001</v>
+        <v>17246.623100000001</v>
       </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>4.9645720000000004</v>
+        <v>4.790728638888889</v>
       </c>
       <c r="G21" s="7">
         <v>82.794399999999996</v>
@@ -2585,15 +2577,15 @@
       <c r="C22" s="25">
         <v>1.25</v>
       </c>
-      <c r="D22" s="12">
+      <c r="D22" s="6">
         <v>42.950499999999998</v>
       </c>
       <c r="E22" s="16">
-        <v>25996.0543</v>
+        <v>25514.443200000002</v>
       </c>
       <c r="F22" s="5">
         <f t="shared" si="0"/>
-        <v>7.2211261944444445</v>
+        <v>7.0873453333333334</v>
       </c>
       <c r="G22" s="7">
         <v>137.96010000000001</v>
@@ -2611,11 +2603,11 @@
         <v>42.506700000000002</v>
       </c>
       <c r="E23" s="16">
-        <v>17064.691699999999</v>
+        <v>17443.039199999999</v>
       </c>
       <c r="F23" s="5">
         <f t="shared" si="0"/>
-        <v>4.7401921388888884</v>
+        <v>4.8452886666666668</v>
       </c>
       <c r="G23" s="5">
         <v>117.2388</v>
@@ -2632,11 +2624,11 @@
         <v>41.526499999999999</v>
       </c>
       <c r="E24" s="16">
-        <v>8641.7073999999993</v>
+        <v>7664.1588000000002</v>
       </c>
       <c r="F24" s="5">
         <f t="shared" si="0"/>
-        <v>2.4004742777777777</v>
+        <v>2.128933</v>
       </c>
       <c r="G24" s="7">
         <v>55.2</v>
@@ -2654,11 +2646,11 @@
         <v>42.469700000000003</v>
       </c>
       <c r="E25" s="16">
-        <v>16326.272999999999</v>
+        <v>17736.298900000002</v>
       </c>
       <c r="F25" s="5">
         <f t="shared" si="0"/>
-        <v>4.535075833333333</v>
+        <v>4.9267496944444451</v>
       </c>
       <c r="G25" s="5">
         <v>117.2388</v>
@@ -2678,11 +2670,11 @@
         <v>42.873399999999997</v>
       </c>
       <c r="E26" s="16">
-        <v>24836.130499999999</v>
+        <v>25344.0589</v>
       </c>
       <c r="F26" s="5">
         <f t="shared" si="0"/>
-        <v>6.898925138888889</v>
+        <v>7.0400163611111113</v>
       </c>
       <c r="G26" s="7">
         <v>137.96010000000001</v>
@@ -2700,11 +2692,11 @@
         <v>42.630499999999998</v>
       </c>
       <c r="E27" s="16">
-        <v>18001.985000000001</v>
+        <v>17575.707299999998</v>
       </c>
       <c r="F27" s="5">
         <f t="shared" si="0"/>
-        <v>5.0005513888888888</v>
+        <v>4.8821409166666658</v>
       </c>
       <c r="G27" s="5">
         <v>117.2388</v>
@@ -2722,11 +2714,11 @@
         <v>42.674599999999998</v>
       </c>
       <c r="E28" s="16">
-        <v>16426.006399999998</v>
+        <v>16103.9485</v>
       </c>
       <c r="F28" s="5">
         <f t="shared" si="0"/>
-        <v>4.5627795555555553</v>
+        <v>4.4733190277777775</v>
       </c>
       <c r="G28" s="7">
         <v>82.794399999999996</v>
@@ -2744,11 +2736,11 @@
         <v>42.784999999999997</v>
       </c>
       <c r="E29" s="16">
-        <v>17347.283800000001</v>
+        <v>17248.306700000001</v>
       </c>
       <c r="F29" s="5">
         <f t="shared" si="0"/>
-        <v>4.8186899444444444</v>
+        <v>4.7911963055555562</v>
       </c>
       <c r="G29" s="7">
         <v>82.794399999999996</v>
@@ -2768,11 +2760,11 @@
         <v>42.680799999999998</v>
       </c>
       <c r="E30" s="16">
-        <v>17049.539199999999</v>
+        <v>17765.7304</v>
       </c>
       <c r="F30" s="5">
         <f t="shared" si="0"/>
-        <v>4.7359831111111106</v>
+        <v>4.9349251111111112</v>
       </c>
       <c r="G30" s="7">
         <v>82.794399999999996</v>
@@ -2790,11 +2782,11 @@
         <v>42.712299999999999</v>
       </c>
       <c r="E31" s="16">
-        <v>17082.367099999999</v>
+        <v>17227.105200000002</v>
       </c>
       <c r="F31" s="5">
         <f t="shared" si="0"/>
-        <v>4.7451019722222219</v>
+        <v>4.7853070000000004</v>
       </c>
       <c r="G31" s="5">
         <v>117.2388</v>
@@ -2812,11 +2804,11 @@
         <v>42.696899999999999</v>
       </c>
       <c r="E32" s="16">
-        <v>16144.677</v>
+        <v>17891.804899999999</v>
       </c>
       <c r="F32" s="5">
         <f t="shared" si="0"/>
-        <v>4.4846325</v>
+        <v>4.9699458055555557</v>
       </c>
       <c r="G32" s="5">
         <v>117.2388</v>
@@ -2834,11 +2826,11 @@
         <v>42.518000000000001</v>
       </c>
       <c r="E33" s="26">
-        <v>21055.982400000001</v>
+        <v>20683.0455</v>
       </c>
       <c r="F33" s="5">
         <f t="shared" si="0"/>
-        <v>5.848884</v>
+        <v>5.7452904166666663</v>
       </c>
       <c r="G33" s="7">
         <v>103.4885</v>
@@ -3021,7 +3013,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3068,19 +3060,13 @@
       <c r="C2" s="25">
         <v>1.25</v>
       </c>
-      <c r="D2" s="4">
-        <v>42.702100000000002</v>
-      </c>
-      <c r="E2" s="14">
-        <v>17217.2395</v>
-      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="14"/>
       <c r="F2" s="19">
         <f t="shared" ref="F2:F18" si="0">E2/3600</f>
-        <v>4.782566527777778</v>
-      </c>
-      <c r="G2" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G2" s="7"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
@@ -3088,19 +3074,13 @@
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6">
-        <v>42.737499999999997</v>
-      </c>
-      <c r="E3" s="15">
-        <v>19008.7209</v>
-      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="15"/>
       <c r="F3" s="19">
         <f t="shared" si="0"/>
-        <v>5.28020025</v>
-      </c>
-      <c r="G3" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
@@ -3108,20 +3088,14 @@
       <c r="C4" s="23">
         <v>1.75</v>
       </c>
-      <c r="D4" s="6">
-        <v>42.5548</v>
-      </c>
-      <c r="E4" s="15">
-        <v>17271.606800000001</v>
-      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="15"/>
       <c r="F4" s="19">
         <f t="shared" si="0"/>
-        <v>4.797668555555556</v>
-      </c>
-      <c r="G4" s="7">
-        <v>117.2388</v>
-      </c>
-      <c r="I4" s="69"/>
+        <v>0</v>
+      </c>
+      <c r="G4" s="7"/>
+      <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="65"/>
@@ -3129,19 +3103,13 @@
       <c r="C5" s="23">
         <v>2</v>
       </c>
-      <c r="D5" s="6">
-        <v>42.728700000000003</v>
-      </c>
-      <c r="E5" s="15">
-        <v>20657.942500000001</v>
-      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="15"/>
       <c r="F5" s="19">
         <f t="shared" si="0"/>
-        <v>5.7383173611111111</v>
-      </c>
-      <c r="G5" s="7">
-        <v>117.2388</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="65"/>
@@ -3151,19 +3119,13 @@
       <c r="C6" s="25">
         <v>1.25</v>
       </c>
-      <c r="D6" s="6">
-        <v>42.873399999999997</v>
-      </c>
-      <c r="E6" s="15">
-        <v>25416.178100000001</v>
-      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="15"/>
       <c r="F6" s="19">
         <f t="shared" si="0"/>
-        <v>7.0600494722222225</v>
-      </c>
-      <c r="G6" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
@@ -3171,19 +3133,13 @@
       <c r="C7" s="23">
         <v>1.5</v>
       </c>
-      <c r="D7" s="6">
-        <v>42.848500000000001</v>
-      </c>
-      <c r="E7" s="15">
-        <v>23798.757699999998</v>
-      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="15"/>
       <c r="F7" s="19">
         <f t="shared" si="0"/>
-        <v>6.6107660277777773</v>
-      </c>
-      <c r="G7" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
@@ -3191,19 +3147,13 @@
       <c r="C8" s="23">
         <v>1.75</v>
       </c>
-      <c r="D8" s="6">
-        <v>42.6203</v>
-      </c>
-      <c r="E8" s="15">
-        <v>16067.453799999999</v>
-      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="15"/>
       <c r="F8" s="19">
         <f t="shared" si="0"/>
-        <v>4.4631816111111107</v>
-      </c>
-      <c r="G8" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="65"/>
@@ -3211,19 +3161,13 @@
       <c r="C9" s="23">
         <v>2</v>
       </c>
-      <c r="D9" s="6">
-        <v>42.587299999999999</v>
-      </c>
-      <c r="E9" s="15">
-        <v>17407.544699999999</v>
-      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="15"/>
       <c r="F9" s="19">
         <f t="shared" si="0"/>
-        <v>4.8354290833333327</v>
-      </c>
-      <c r="G9" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="65"/>
@@ -3233,19 +3177,13 @@
       <c r="C10" s="25">
         <v>1.25</v>
       </c>
-      <c r="D10" s="6">
-        <v>42.3277</v>
-      </c>
-      <c r="E10" s="15">
-        <v>15134.318600000001</v>
-      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="15"/>
       <c r="F10" s="19">
         <f t="shared" si="0"/>
-        <v>4.2039773888888892</v>
-      </c>
-      <c r="G10" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
@@ -3253,19 +3191,13 @@
       <c r="C11" s="23">
         <v>1.5</v>
       </c>
-      <c r="D11" s="6">
-        <v>42.418700000000001</v>
-      </c>
-      <c r="E11" s="15">
-        <v>17504.587299999999</v>
-      </c>
+      <c r="D11" s="6"/>
+      <c r="E11" s="15"/>
       <c r="F11" s="19">
         <f t="shared" si="0"/>
-        <v>4.8623853611111105</v>
-      </c>
-      <c r="G11" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
@@ -3273,19 +3205,13 @@
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
-      <c r="D12" s="6">
-        <v>41.464199999999998</v>
-      </c>
-      <c r="E12" s="15">
-        <v>8568.4732999999997</v>
-      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="15"/>
       <c r="F12" s="19">
         <f t="shared" si="0"/>
-        <v>2.3801314722222222</v>
-      </c>
-      <c r="G12" s="7">
-        <v>27.621300000000002</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="65"/>
@@ -3293,19 +3219,13 @@
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="6">
-        <v>42.8294</v>
-      </c>
-      <c r="E13" s="15">
-        <v>23575.140299999999</v>
-      </c>
+      <c r="D13" s="6"/>
+      <c r="E13" s="15"/>
       <c r="F13" s="19">
         <f t="shared" si="0"/>
-        <v>6.5486500833333334</v>
-      </c>
-      <c r="G13" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="65"/>
@@ -3315,19 +3235,13 @@
       <c r="C14" s="25">
         <v>1.25</v>
       </c>
-      <c r="D14" s="6">
-        <v>42.453299999999999</v>
-      </c>
-      <c r="E14" s="16">
-        <v>15651.1404</v>
-      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="16"/>
       <c r="F14" s="19">
         <f t="shared" si="0"/>
-        <v>4.3475390000000003</v>
-      </c>
-      <c r="G14" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="65"/>
@@ -3335,19 +3249,13 @@
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
-      <c r="D15" s="6">
-        <v>42.844499999999996</v>
-      </c>
-      <c r="E15" s="15">
-        <v>16197.331099999999</v>
-      </c>
+      <c r="D15" s="6"/>
+      <c r="E15" s="15"/>
       <c r="F15" s="19">
         <f t="shared" si="0"/>
-        <v>4.4992586388888887</v>
-      </c>
-      <c r="G15" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
@@ -3355,19 +3263,13 @@
       <c r="C16" s="23">
         <v>1.75</v>
       </c>
-      <c r="D16" s="6">
-        <v>42.287599999999998</v>
-      </c>
-      <c r="E16" s="15">
-        <v>15399.1762</v>
-      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="15"/>
       <c r="F16" s="19">
         <f t="shared" si="0"/>
-        <v>4.2775489444444448</v>
-      </c>
-      <c r="G16" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
@@ -3375,19 +3277,13 @@
       <c r="C17" s="23">
         <v>2</v>
       </c>
-      <c r="D17" s="6">
-        <v>42.500799999999998</v>
-      </c>
-      <c r="E17" s="16">
-        <v>16000.301600000001</v>
-      </c>
+      <c r="D17" s="6"/>
+      <c r="E17" s="16"/>
       <c r="F17" s="19">
         <f t="shared" si="0"/>
-        <v>4.444528222222222</v>
-      </c>
-      <c r="G17" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
@@ -3399,19 +3295,13 @@
       <c r="C18" s="25">
         <v>1.25</v>
       </c>
-      <c r="D18" s="6">
-        <v>42.648099999999999</v>
-      </c>
-      <c r="E18" s="16">
-        <v>17592.232599999999</v>
-      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="16"/>
       <c r="F18" s="19">
         <f t="shared" si="0"/>
-        <v>4.8867312777777778</v>
-      </c>
-      <c r="G18" s="7">
-        <v>117.2388</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
@@ -3419,19 +3309,13 @@
       <c r="C19" s="23">
         <v>1.5</v>
       </c>
-      <c r="D19" s="6">
-        <v>42.956299999999999</v>
-      </c>
-      <c r="E19" s="16">
-        <v>25320.490600000001</v>
-      </c>
+      <c r="D19" s="6"/>
+      <c r="E19" s="16"/>
       <c r="F19" s="19">
         <f>E19/3600</f>
-        <v>7.0334696111111112</v>
-      </c>
-      <c r="G19" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
@@ -3439,19 +3323,13 @@
       <c r="C20" s="23">
         <v>1.75</v>
       </c>
-      <c r="D20" s="6">
-        <v>42.490900000000003</v>
-      </c>
-      <c r="E20" s="16">
-        <v>15511.254499999999</v>
-      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="16"/>
       <c r="F20" s="19">
         <f t="shared" ref="F20:F33" si="1">E20/3600</f>
-        <v>4.3086818055555556</v>
-      </c>
-      <c r="G20" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
@@ -3459,19 +3337,13 @@
       <c r="C21" s="23">
         <v>2</v>
       </c>
-      <c r="D21" s="6">
-        <v>42.452800000000003</v>
-      </c>
-      <c r="E21" s="16">
-        <v>15414.6432</v>
-      </c>
+      <c r="D21" s="6"/>
+      <c r="E21" s="16"/>
       <c r="F21" s="19">
         <f t="shared" si="1"/>
-        <v>4.2818453333333331</v>
-      </c>
-      <c r="G21" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
@@ -3481,19 +3353,13 @@
       <c r="C22" s="25">
         <v>1.25</v>
       </c>
-      <c r="D22" s="6">
-        <v>42.461300000000001</v>
-      </c>
-      <c r="E22" s="16">
-        <v>14137.963900000001</v>
-      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="16"/>
       <c r="F22" s="19">
         <f t="shared" si="1"/>
-        <v>3.9272121944444445</v>
-      </c>
-      <c r="G22" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
@@ -3501,19 +3367,13 @@
       <c r="C23" s="23">
         <v>1.5</v>
       </c>
-      <c r="D23" s="6">
-        <v>42.7879</v>
-      </c>
-      <c r="E23" s="16">
-        <v>25338.7857</v>
-      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="16"/>
       <c r="F23" s="19">
         <f t="shared" si="1"/>
-        <v>7.0385515833333336</v>
-      </c>
-      <c r="G23" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
@@ -3521,19 +3381,13 @@
       <c r="C24" s="23">
         <v>1.75</v>
       </c>
-      <c r="D24" s="6">
-        <v>42.816600000000001</v>
-      </c>
-      <c r="E24" s="16">
-        <v>25830.7084</v>
-      </c>
+      <c r="D24" s="6"/>
+      <c r="E24" s="16"/>
       <c r="F24" s="19">
         <f t="shared" si="1"/>
-        <v>7.1751967777777779</v>
-      </c>
-      <c r="G24" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
@@ -3541,19 +3395,13 @@
       <c r="C25" s="23">
         <v>2</v>
       </c>
-      <c r="D25" s="6">
-        <v>42.893900000000002</v>
-      </c>
-      <c r="E25" s="16">
-        <v>22675.105200000002</v>
-      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="16"/>
       <c r="F25" s="19">
         <f t="shared" si="1"/>
-        <v>6.2986403333333341</v>
-      </c>
-      <c r="G25" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
@@ -3563,19 +3411,13 @@
       <c r="C26" s="25">
         <v>1.25</v>
       </c>
-      <c r="D26" s="6">
-        <v>42.756799999999998</v>
-      </c>
-      <c r="E26" s="16">
-        <v>17946.270400000001</v>
-      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="16"/>
       <c r="F26" s="19">
         <f t="shared" si="1"/>
-        <v>4.9850751111111116</v>
-      </c>
-      <c r="G26" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="35"/>
@@ -3583,19 +3425,13 @@
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
-      <c r="D27" s="12">
-        <v>43.082599999999999</v>
-      </c>
-      <c r="E27" s="16">
-        <v>23625.376100000001</v>
-      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="16"/>
       <c r="F27" s="19">
         <f t="shared" si="1"/>
-        <v>6.5626044722222225</v>
-      </c>
-      <c r="G27" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="35"/>
@@ -3603,19 +3439,13 @@
       <c r="C28" s="23">
         <v>1.75</v>
       </c>
-      <c r="D28" s="6">
-        <v>42.710799999999999</v>
-      </c>
-      <c r="E28" s="16">
-        <v>16154.835499999999</v>
-      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="16"/>
       <c r="F28" s="19">
         <f t="shared" si="1"/>
-        <v>4.4874543055555556</v>
-      </c>
-      <c r="G28" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="35"/>
@@ -3623,19 +3453,13 @@
       <c r="C29" s="23">
         <v>2</v>
       </c>
-      <c r="D29" s="6">
-        <v>42.746400000000001</v>
-      </c>
-      <c r="E29" s="16">
-        <v>16132.570599999999</v>
-      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="16"/>
       <c r="F29" s="19">
         <f t="shared" si="1"/>
-        <v>4.4812696111111112</v>
-      </c>
-      <c r="G29" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="35"/>
@@ -3645,19 +3469,13 @@
       <c r="C30" s="25">
         <v>1.25</v>
       </c>
-      <c r="D30" s="6">
-        <v>42.915700000000001</v>
-      </c>
-      <c r="E30" s="16">
-        <v>23288.329099999999</v>
-      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="16"/>
       <c r="F30" s="19">
         <f t="shared" si="1"/>
-        <v>6.4689803055555553</v>
-      </c>
-      <c r="G30" s="7">
-        <v>137.96010000000001</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="35"/>
@@ -3665,19 +3483,13 @@
       <c r="C31" s="23">
         <v>1.5</v>
       </c>
-      <c r="D31" s="6">
-        <v>42.592100000000002</v>
-      </c>
-      <c r="E31" s="16">
-        <v>18890.779900000001</v>
-      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="16"/>
       <c r="F31" s="19">
         <f t="shared" si="1"/>
-        <v>5.2474388611111111</v>
-      </c>
-      <c r="G31" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="35"/>
@@ -3685,19 +3497,13 @@
       <c r="C32" s="23">
         <v>1.75</v>
       </c>
-      <c r="D32" s="6">
-        <v>42.393799999999999</v>
-      </c>
-      <c r="E32" s="16">
-        <v>14328.2937</v>
-      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="16"/>
       <c r="F32" s="19">
         <f t="shared" si="1"/>
-        <v>3.9800815833333334</v>
-      </c>
-      <c r="G32" s="7">
-        <v>103.4885</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="36"/>
@@ -3705,19 +3511,13 @@
       <c r="C33" s="23">
         <v>2</v>
       </c>
-      <c r="D33" s="6">
-        <v>42.602400000000003</v>
-      </c>
-      <c r="E33" s="16">
-        <v>15981.097599999999</v>
-      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="16"/>
       <c r="F33" s="19">
         <f t="shared" si="1"/>
-        <v>4.4391937777777777</v>
-      </c>
-      <c r="G33" s="7">
-        <v>82.794399999999996</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G33" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3742,7 +3542,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3791,7 +3591,10 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="14"/>
-      <c r="F2" s="5"/>
+      <c r="F2" s="5">
+        <f>E2/3600</f>
+        <v>0</v>
+      </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -3802,7 +3605,10 @@
       </c>
       <c r="D3" s="6"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="7"/>
+      <c r="F3" s="5">
+        <f t="shared" ref="F3:F33" si="0">E3/3600</f>
+        <v>0</v>
+      </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
@@ -3813,7 +3619,10 @@
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="15"/>
-      <c r="F4" s="7"/>
+      <c r="F4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3824,7 +3633,10 @@
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="15"/>
-      <c r="F5" s="7"/>
+      <c r="F5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
@@ -3837,7 +3649,10 @@
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="15"/>
-      <c r="F6" s="7"/>
+      <c r="F6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G6" s="7"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -3848,7 +3663,10 @@
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="15"/>
-      <c r="F7" s="7"/>
+      <c r="F7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -3859,7 +3677,10 @@
       </c>
       <c r="D8" s="6"/>
       <c r="E8" s="15"/>
-      <c r="F8" s="7"/>
+      <c r="F8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -3870,7 +3691,10 @@
       </c>
       <c r="D9" s="6"/>
       <c r="E9" s="15"/>
-      <c r="F9" s="7"/>
+      <c r="F9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -3883,7 +3707,10 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="15"/>
-      <c r="F10" s="7"/>
+      <c r="F10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -3894,7 +3721,10 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="15"/>
-      <c r="F11" s="7"/>
+      <c r="F11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -3905,7 +3735,10 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="15"/>
-      <c r="F12" s="7"/>
+      <c r="F12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -3916,7 +3749,10 @@
       </c>
       <c r="D13" s="6"/>
       <c r="E13" s="15"/>
-      <c r="F13" s="7"/>
+      <c r="F13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G13" s="7"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -3929,7 +3765,10 @@
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="16"/>
-      <c r="F14" s="7"/>
+      <c r="F14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -3940,7 +3779,10 @@
       </c>
       <c r="D15" s="6"/>
       <c r="E15" s="15"/>
-      <c r="F15" s="7"/>
+      <c r="F15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -3951,7 +3793,10 @@
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="15"/>
-      <c r="F16" s="7"/>
+      <c r="F16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -3962,7 +3807,10 @@
       </c>
       <c r="D17" s="6"/>
       <c r="E17" s="16"/>
-      <c r="F17" s="7"/>
+      <c r="F17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
@@ -3977,7 +3825,10 @@
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="16"/>
-      <c r="F18" s="19"/>
+      <c r="F18" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -3988,7 +3839,10 @@
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="16"/>
-      <c r="F19" s="19"/>
+      <c r="F19" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -3999,7 +3853,10 @@
       </c>
       <c r="D20" s="6"/>
       <c r="E20" s="16"/>
-      <c r="F20" s="19"/>
+      <c r="F20" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
@@ -4010,7 +3867,10 @@
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="16"/>
-      <c r="F21" s="19"/>
+      <c r="F21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -4023,7 +3883,10 @@
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="16"/>
-      <c r="F22" s="19"/>
+      <c r="F22" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -4034,7 +3897,10 @@
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="16"/>
-      <c r="F23" s="19"/>
+      <c r="F23" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
@@ -4045,7 +3911,10 @@
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="16"/>
-      <c r="F24" s="19"/>
+      <c r="F24" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
@@ -4056,7 +3925,10 @@
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="16"/>
-      <c r="F25" s="19"/>
+      <c r="F25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
@@ -4069,7 +3941,10 @@
       </c>
       <c r="D26" s="6"/>
       <c r="E26" s="16"/>
-      <c r="F26" s="19"/>
+      <c r="F26" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
@@ -4080,7 +3955,10 @@
       </c>
       <c r="D27" s="6"/>
       <c r="E27" s="16"/>
-      <c r="F27" s="19"/>
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
@@ -4091,7 +3969,10 @@
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="16"/>
-      <c r="F28" s="19"/>
+      <c r="F28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -4102,7 +3983,10 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="16"/>
-      <c r="F29" s="19"/>
+      <c r="F29" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
@@ -4115,7 +3999,10 @@
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="16"/>
-      <c r="F30" s="19"/>
+      <c r="F30" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
@@ -4126,7 +4013,10 @@
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="16"/>
-      <c r="F31" s="19"/>
+      <c r="F31" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
@@ -4137,7 +4027,10 @@
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="16"/>
-      <c r="F32" s="19"/>
+      <c r="F32" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
@@ -4148,7 +4041,10 @@
       </c>
       <c r="D33" s="6"/>
       <c r="E33" s="16"/>
-      <c r="F33" s="19"/>
+      <c r="F33" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="G33" s="7"/>
     </row>
     <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4176,7 +4072,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4219,7 +4115,10 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5">
+        <f>D2/3600</f>
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
       <c r="G2" s="28"/>
       <c r="H2" s="10"/>
@@ -4231,7 +4130,10 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="5"/>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E17" si="0">D3/3600</f>
+        <v>0</v>
+      </c>
       <c r="F3" s="7"/>
       <c r="G3" s="28"/>
       <c r="H3" s="10"/>
@@ -4243,7 +4145,10 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="5"/>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F4" s="7"/>
       <c r="G4" s="28"/>
       <c r="H4" s="10"/>
@@ -4255,7 +4160,10 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="5"/>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="28"/>
       <c r="H5" s="10"/>
@@ -4269,7 +4177,10 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="5"/>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="28"/>
       <c r="H6" s="10"/>
@@ -4281,7 +4192,10 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="5"/>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="28"/>
       <c r="H7" s="10"/>
@@ -4293,7 +4207,10 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="5"/>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="28"/>
       <c r="H8" s="10"/>
@@ -4305,7 +4222,10 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="28"/>
       <c r="H9" s="10"/>
@@ -4319,7 +4239,10 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="28"/>
       <c r="H10" s="10"/>
@@ -4331,7 +4254,10 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="28"/>
       <c r="H11" s="10"/>
@@ -4343,7 +4269,10 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="5"/>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="5"/>
       <c r="G12" s="28"/>
       <c r="H12" s="10"/>
@@ -4355,7 +4284,10 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="5"/>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="28"/>
       <c r="H13" s="10"/>
@@ -4369,7 +4301,10 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="5"/>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="28"/>
       <c r="H14" s="10"/>
@@ -4381,7 +4316,10 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="5"/>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="28"/>
       <c r="H15" s="10"/>
@@ -4393,7 +4331,10 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="5"/>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="28"/>
       <c r="H16" s="10"/>
@@ -4405,7 +4346,10 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="5"/>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="28"/>
       <c r="H17" s="10"/>
@@ -4725,7 +4669,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="E2" sqref="E2:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4767,7 +4711,10 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5">
+        <f>D2/3600</f>
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -4777,7 +4724,10 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E17" si="0">D3/3600</f>
+        <v>0</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -4787,7 +4737,10 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -4797,7 +4750,10 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -4809,7 +4765,10 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -4819,7 +4778,10 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -4829,7 +4791,10 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -4839,7 +4804,10 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -4851,7 +4819,10 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -4861,7 +4832,10 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -4871,7 +4845,10 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -4881,7 +4858,10 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -4893,7 +4873,10 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -4903,7 +4886,10 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -4913,7 +4899,10 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -4923,7 +4912,10 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -5095,7 +5087,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5137,7 +5129,10 @@
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="14"/>
-      <c r="E2" s="5"/>
+      <c r="E2" s="5">
+        <f>D2/3600</f>
+        <v>0</v>
+      </c>
       <c r="F2" s="5"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -5147,7 +5142,10 @@
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="15"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="5">
+        <f t="shared" ref="E3:E17" si="0">D3/3600</f>
+        <v>0</v>
+      </c>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -5157,7 +5155,10 @@
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="15"/>
-      <c r="E4" s="7"/>
+      <c r="E4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -5167,7 +5168,10 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="15"/>
-      <c r="E5" s="7"/>
+      <c r="E5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -5179,7 +5183,10 @@
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="15"/>
-      <c r="E6" s="7"/>
+      <c r="E6" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -5189,7 +5196,10 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="15"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -5199,7 +5209,10 @@
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="15"/>
-      <c r="E8" s="7"/>
+      <c r="E8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -5209,7 +5222,10 @@
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="15"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -5221,7 +5237,10 @@
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="15"/>
-      <c r="E10" s="7"/>
+      <c r="E10" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -5231,7 +5250,10 @@
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="15"/>
-      <c r="E11" s="7"/>
+      <c r="E11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -5241,7 +5263,10 @@
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="15"/>
-      <c r="E12" s="7"/>
+      <c r="E12" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -5251,7 +5276,10 @@
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="15"/>
-      <c r="E13" s="7"/>
+      <c r="E13" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -5263,7 +5291,10 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="16"/>
-      <c r="E14" s="7"/>
+      <c r="E14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -5273,7 +5304,10 @@
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="15"/>
-      <c r="E15" s="7"/>
+      <c r="E15" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -5283,7 +5317,10 @@
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="15"/>
-      <c r="E16" s="7"/>
+      <c r="E16" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -5293,7 +5330,10 @@
       </c>
       <c r="C17" s="6"/>
       <c r="D17" s="16"/>
-      <c r="E17" s="7"/>
+      <c r="E17" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update final opus-base hyp search simple adapt wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2338" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABD1CA7A-BA30-4836-AF26-1F7B55760102}"/>
+  <xr:revisionPtr revIDLastSave="2349" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF08B928-C48C-4B44-967E-DAC7B31DC1AC}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>Weight</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Weighted Proportion</t>
-  </si>
-  <si>
-    <t>RERUN</t>
   </si>
 </sst>
 </file>
@@ -574,6 +571,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -595,12 +649,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,57 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1008,13 +1005,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1036,9 +1033,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1058,9 +1055,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1080,9 +1077,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1102,9 +1099,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44">
+      <c r="A6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1126,9 +1123,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1148,9 +1145,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1170,9 +1167,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1192,9 +1189,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1216,9 +1213,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1238,9 +1235,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1260,9 +1257,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1282,9 +1279,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44">
+      <c r="A14" s="57"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1306,9 +1303,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1328,9 +1325,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1350,9 +1347,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1372,11 +1369,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="34">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1396,9 +1393,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1418,9 +1415,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1440,9 +1437,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1462,11 +1459,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44">
+      <c r="A22" s="57"/>
+      <c r="B22" s="61">
         <v>0.75</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1486,9 +1483,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1507,9 +1504,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1529,9 +1526,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1551,11 +1548,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61">
         <v>0.5</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1575,9 +1572,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1597,9 +1594,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1619,9 +1616,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1641,11 +1638,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="44">
+      <c r="A30" s="57"/>
+      <c r="B30" s="61">
         <v>0.25</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1665,9 +1662,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1687,9 +1684,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1709,9 +1706,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1731,13 +1728,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="63">
         <v>0.1</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="63">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1759,9 +1756,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1781,9 +1778,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1803,9 +1800,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1825,14 +1822,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1849,12 +1846,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="48" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1871,13 +1868,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1899,9 +1896,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1923,11 +1920,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1949,9 +1946,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1973,14 +1970,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1997,12 +1994,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="48" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2019,12 +2016,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2051,13 +2048,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2074,6 +2064,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2085,7 +2082,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2357,16 +2354,20 @@
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="6">
+        <v>42.600499999999997</v>
+      </c>
+      <c r="E12" s="15">
+        <v>16025.9216</v>
+      </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5"/>
-      <c r="H12" s="28" t="s">
-        <v>24</v>
-      </c>
+        <v>4.4516448888888887</v>
+      </c>
+      <c r="G12" s="7">
+        <v>82.794399999999996</v>
+      </c>
+      <c r="H12" s="28"/>
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -2375,16 +2376,20 @@
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="6">
+        <v>42.482199999999999</v>
+      </c>
+      <c r="E13" s="15">
+        <v>20594.264599999999</v>
+      </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="7"/>
-      <c r="H13" s="28" t="s">
-        <v>24</v>
-      </c>
+        <v>5.7206290555555555</v>
+      </c>
+      <c r="G13" s="7">
+        <v>137.96010000000001</v>
+      </c>
+      <c r="H13" s="28"/>
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
@@ -2478,7 +2483,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2504,7 +2509,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2526,7 +2531,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2548,7 +2553,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2570,14 +2575,14 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
       <c r="C22" s="25">
         <v>1.25</v>
       </c>
-      <c r="D22" s="6">
+      <c r="D22" s="12">
         <v>42.950499999999998</v>
       </c>
       <c r="E22" s="16">
@@ -2594,7 +2599,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2615,7 +2620,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2637,7 +2642,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2659,7 +2664,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2683,7 +2688,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2705,7 +2710,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2727,7 +2732,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2749,7 +2754,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2773,7 +2778,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2795,7 +2800,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2817,7 +2822,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3286,7 +3291,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3304,7 +3309,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3318,7 +3323,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3332,7 +3337,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3346,7 +3351,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3362,7 +3367,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3376,7 +3381,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3390,7 +3395,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3404,7 +3409,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3420,7 +3425,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3434,7 +3439,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3448,7 +3453,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3462,7 +3467,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3478,7 +3483,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3492,7 +3497,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3506,7 +3511,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3521,16 +3526,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3814,7 +3819,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -3832,7 +3837,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3846,7 +3851,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3860,7 +3865,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3874,7 +3879,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -3890,7 +3895,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3904,7 +3909,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3918,7 +3923,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3932,7 +3937,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -3948,7 +3953,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3962,7 +3967,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3976,7 +3981,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3990,7 +3995,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4006,7 +4011,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4020,7 +4025,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4034,7 +4039,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4051,16 +4056,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5504,12 +5509,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5742,17 +5746,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5777,18 +5791,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update opus-big simple adapt wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -571,6 +571,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,24 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -626,39 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,13 +1005,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="36">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1033,9 +1033,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1055,9 +1055,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1077,9 +1077,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1099,9 +1099,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61">
+      <c r="A6" s="38"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1123,9 +1123,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1145,9 +1145,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1167,9 +1167,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1189,9 +1189,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61">
+      <c r="A10" s="38"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1213,9 +1213,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1235,9 +1235,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1257,9 +1257,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1279,9 +1279,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61">
+      <c r="A14" s="38"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1303,9 +1303,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1325,9 +1325,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1347,9 +1347,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1369,11 +1369,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="57"/>
-      <c r="B18" s="53">
+      <c r="A18" s="38"/>
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1393,9 +1393,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="57"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="61"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1415,9 +1415,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="57"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="61"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1437,9 +1437,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="61"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1459,11 +1459,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="57"/>
-      <c r="B22" s="61">
+      <c r="A22" s="38"/>
+      <c r="B22" s="44">
         <v>0.75</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1483,9 +1483,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="57"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1504,9 +1504,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="57"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1526,9 +1526,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1548,11 +1548,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="61">
+      <c r="A26" s="38"/>
+      <c r="B26" s="44">
         <v>0.5</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1572,9 +1572,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="57"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1594,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1616,9 +1616,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1638,11 +1638,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="61">
+      <c r="A30" s="38"/>
+      <c r="B30" s="44">
         <v>0.25</v>
       </c>
-      <c r="C30" s="61"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1662,9 +1662,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1684,9 +1684,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1706,9 +1706,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1728,13 +1728,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="46">
         <v>0.1</v>
       </c>
-      <c r="C34" s="63">
+      <c r="C34" s="46">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1756,9 +1756,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1778,9 +1778,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="39"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1800,9 +1800,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1822,14 +1822,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1846,12 +1846,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1868,13 +1868,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1896,9 +1896,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="52"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1920,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="46" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="47"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1946,9 +1946,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1970,14 +1970,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="36"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1994,12 +1994,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="38"/>
-      <c r="B45" s="40" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2016,12 +2016,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2048,6 +2048,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2064,13 +2071,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2082,7 +2082,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2483,7 +2483,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2509,7 +2509,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2531,7 +2531,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2553,7 +2553,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2575,7 +2575,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2620,7 +2620,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2642,7 +2642,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2664,7 +2664,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2710,7 +2710,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2732,7 +2732,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2754,7 +2754,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2800,7 +2800,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2822,7 +2822,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3291,7 +3291,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3309,7 +3309,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3323,7 +3323,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3337,7 +3337,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3351,7 +3351,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3367,7 +3367,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3381,7 +3381,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3395,7 +3395,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3409,7 +3409,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3425,7 +3425,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3439,7 +3439,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3453,7 +3453,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3467,7 +3467,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3483,7 +3483,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3497,7 +3497,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3511,7 +3511,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3526,16 +3526,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3819,7 +3819,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -3837,7 +3837,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3851,7 +3851,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3865,7 +3865,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3879,7 +3879,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -3895,7 +3895,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3909,7 +3909,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3923,7 +3923,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3937,7 +3937,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -3953,7 +3953,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3967,7 +3967,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3981,7 +3981,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3995,7 +3995,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4011,7 +4011,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4025,7 +4025,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4039,7 +4039,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4056,16 +4056,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5509,11 +5509,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5746,27 +5747,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5791,9 +5782,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add first batch of opus-base AoN wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2349" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF08B928-C48C-4B44-967E-DAC7B31DC1AC}"/>
+  <xr:revisionPtr revIDLastSave="2443" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95DD70C4-41FE-45B5-BAC8-3559C442D11F}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
   <si>
     <t>Weight</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Weighted Proportion</t>
+  </si>
+  <si>
+    <t>RERUN</t>
   </si>
 </sst>
 </file>
@@ -571,6 +574,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -592,12 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,57 +662,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,13 +1008,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1033,9 +1036,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1055,9 +1058,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1077,9 +1080,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1099,9 +1102,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44">
+      <c r="A6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1123,9 +1126,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1145,9 +1148,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1167,9 +1170,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1189,9 +1192,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1213,9 +1216,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1235,9 +1238,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1257,9 +1260,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1279,9 +1282,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44">
+      <c r="A14" s="57"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1303,9 +1306,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1325,9 +1328,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1347,9 +1350,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1369,11 +1372,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="34">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1393,9 +1396,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1415,9 +1418,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1437,9 +1440,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1459,11 +1462,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44">
+      <c r="A22" s="57"/>
+      <c r="B22" s="61">
         <v>0.75</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1483,9 +1486,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1504,9 +1507,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1526,9 +1529,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1548,11 +1551,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61">
         <v>0.5</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1572,9 +1575,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1597,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1616,9 +1619,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1638,11 +1641,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="44">
+      <c r="A30" s="57"/>
+      <c r="B30" s="61">
         <v>0.25</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1662,9 +1665,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1684,9 +1687,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1706,9 +1709,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1728,13 +1731,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="63">
         <v>0.1</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="63">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1756,9 +1759,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1778,9 +1781,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1800,9 +1803,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1822,14 +1825,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1846,12 +1849,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="48" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1868,13 +1871,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1896,9 +1899,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1923,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1946,9 +1949,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1970,14 +1973,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1994,12 +1997,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="48" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2016,12 +2019,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2048,13 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2071,6 +2067,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2081,7 +2084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{123C20E6-94C4-4B99-8775-24B7DED1396E}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
@@ -2483,7 +2486,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2509,7 +2512,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2531,7 +2534,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2553,7 +2556,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2575,7 +2578,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2599,7 +2602,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2620,7 +2623,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2642,7 +2645,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2664,7 +2667,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2688,7 +2691,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2710,7 +2713,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2732,7 +2735,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2754,7 +2757,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2778,7 +2781,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2800,7 +2803,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2822,7 +2825,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3017,8 +3020,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B44CA5E-D6A9-491D-9F24-D323A0E66CBD}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I14:I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3065,13 +3068,19 @@
       <c r="C2" s="25">
         <v>1.25</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="4">
+        <v>42.786499999999997</v>
+      </c>
+      <c r="E2" s="14">
+        <v>25347.2356</v>
+      </c>
       <c r="F2" s="19">
         <f t="shared" ref="F2:F18" si="0">E2/3600</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="7"/>
+        <v>7.0408987777777776</v>
+      </c>
+      <c r="G2" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
@@ -3079,13 +3088,19 @@
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="15"/>
+      <c r="D3" s="6">
+        <v>42.887900000000002</v>
+      </c>
+      <c r="E3" s="15">
+        <v>25510.771799999999</v>
+      </c>
       <c r="F3" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G3" s="7"/>
+        <v>7.0863255000000001</v>
+      </c>
+      <c r="G3" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
@@ -3093,13 +3108,19 @@
       <c r="C4" s="23">
         <v>1.75</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="6">
+        <v>42.514000000000003</v>
+      </c>
+      <c r="E4" s="15">
+        <v>15533.8976</v>
+      </c>
       <c r="F4" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="7"/>
+        <v>4.3149715555555552</v>
+      </c>
+      <c r="G4" s="7">
+        <v>103.4885</v>
+      </c>
       <c r="I4" s="32"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -3108,13 +3129,19 @@
       <c r="C5" s="23">
         <v>2</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="6">
+        <v>42.667000000000002</v>
+      </c>
+      <c r="E5" s="15">
+        <v>21958.950099999998</v>
+      </c>
       <c r="F5" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>6.0997083611111105</v>
+      </c>
+      <c r="G5" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="65"/>
@@ -3124,13 +3151,19 @@
       <c r="C6" s="25">
         <v>1.25</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="6">
+        <v>42.4223</v>
+      </c>
+      <c r="E6" s="15">
+        <v>14082.0273</v>
+      </c>
       <c r="F6" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
+        <v>3.9116742499999999</v>
+      </c>
+      <c r="G6" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
@@ -3138,13 +3171,19 @@
       <c r="C7" s="23">
         <v>1.5</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="6">
+        <v>42.667099999999998</v>
+      </c>
+      <c r="E7" s="15">
+        <v>16098.758</v>
+      </c>
       <c r="F7" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="7"/>
+        <v>4.4718772222222221</v>
+      </c>
+      <c r="G7" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
@@ -3159,6 +3198,9 @@
         <v>0</v>
       </c>
       <c r="G8" s="7"/>
+      <c r="H8" s="30" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="65"/>
@@ -3173,6 +3215,9 @@
         <v>0</v>
       </c>
       <c r="G9" s="7"/>
+      <c r="H9" s="30" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="65"/>
@@ -3182,13 +3227,19 @@
       <c r="C10" s="25">
         <v>1.25</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="6">
+        <v>42.213099999999997</v>
+      </c>
+      <c r="E10" s="15">
+        <v>12302.7181</v>
+      </c>
       <c r="F10" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="7"/>
+        <v>3.4174216944444447</v>
+      </c>
+      <c r="G10" s="7">
+        <v>55.2</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
@@ -3196,13 +3247,19 @@
       <c r="C11" s="23">
         <v>1.5</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="6">
+        <v>42.790999999999997</v>
+      </c>
+      <c r="E11" s="15">
+        <v>23377.747599999999</v>
+      </c>
       <c r="F11" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="7"/>
+        <v>6.4938187777777774</v>
+      </c>
+      <c r="G11" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
@@ -3210,13 +3267,19 @@
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="6">
+        <v>42.812800000000003</v>
+      </c>
+      <c r="E12" s="15">
+        <v>23655.583500000001</v>
+      </c>
       <c r="F12" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="7"/>
+        <v>6.5709954166666664</v>
+      </c>
+      <c r="G12" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="65"/>
@@ -3224,13 +3287,19 @@
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="6">
+        <v>41.351100000000002</v>
+      </c>
+      <c r="E13" s="15">
+        <v>7633.6194999999998</v>
+      </c>
       <c r="F13" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="7"/>
+        <v>2.1204498611111111</v>
+      </c>
+      <c r="G13" s="7">
+        <v>55.2</v>
+      </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="65"/>
@@ -3247,6 +3316,9 @@
         <v>0</v>
       </c>
       <c r="G14" s="7"/>
+      <c r="H14" s="30" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="65"/>
@@ -3254,13 +3326,19 @@
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="15"/>
+      <c r="D15" s="6">
+        <v>42.631599999999999</v>
+      </c>
+      <c r="E15" s="15">
+        <v>17734.6571</v>
+      </c>
       <c r="F15" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="7"/>
+        <v>4.9262936388888887</v>
+      </c>
+      <c r="G15" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
@@ -3268,13 +3346,19 @@
       <c r="C16" s="23">
         <v>1.75</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="6">
+        <v>42.515000000000001</v>
+      </c>
+      <c r="E16" s="15">
+        <v>17622.741099999999</v>
+      </c>
       <c r="F16" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="7"/>
+        <v>4.8952058611111111</v>
+      </c>
+      <c r="G16" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
@@ -3282,16 +3366,22 @@
       <c r="C17" s="23">
         <v>2</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="6">
+        <v>42.253300000000003</v>
+      </c>
+      <c r="E17" s="16">
+        <v>16089.025799999999</v>
+      </c>
       <c r="F17" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="7"/>
+        <v>4.4691738333333335</v>
+      </c>
+      <c r="G17" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3300,242 +3390,338 @@
       <c r="C18" s="25">
         <v>1.25</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="16"/>
+      <c r="D18" s="6">
+        <v>42.648099999999999</v>
+      </c>
+      <c r="E18" s="16">
+        <v>15983.9521</v>
+      </c>
       <c r="F18" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="7"/>
+        <v>4.4399866944444444</v>
+      </c>
+      <c r="G18" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="6">
+        <v>42.956299999999999</v>
+      </c>
+      <c r="E19" s="16">
+        <v>25439.283500000001</v>
+      </c>
       <c r="F19" s="19">
         <f>E19/3600</f>
-        <v>0</v>
-      </c>
-      <c r="G19" s="7"/>
+        <v>7.0664676388888896</v>
+      </c>
+      <c r="G19" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="6">
+        <v>42.490900000000003</v>
+      </c>
+      <c r="E20" s="16">
+        <v>15647.784</v>
+      </c>
       <c r="F20" s="19">
         <f t="shared" ref="F20:F33" si="1">E20/3600</f>
-        <v>0</v>
-      </c>
-      <c r="G20" s="7"/>
+        <v>4.3466066666666663</v>
+      </c>
+      <c r="G20" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="6">
+        <v>42.452800000000003</v>
+      </c>
+      <c r="E21" s="16">
+        <v>14312.3127</v>
+      </c>
       <c r="F21" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="7"/>
+        <v>3.9756424166666666</v>
+      </c>
+      <c r="G21" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
       <c r="C22" s="25">
         <v>1.25</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="6">
+        <v>42.461300000000001</v>
+      </c>
+      <c r="E22" s="16">
+        <v>15660.638000000001</v>
+      </c>
       <c r="F22" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="7"/>
+        <v>4.3501772222222224</v>
+      </c>
+      <c r="G22" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="6">
+        <v>42.7879</v>
+      </c>
+      <c r="E23" s="16">
+        <v>25494.8253</v>
+      </c>
       <c r="F23" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>7.0818959166666664</v>
+      </c>
+      <c r="G23" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="16"/>
+      <c r="D24" s="6">
+        <v>42.816600000000001</v>
+      </c>
+      <c r="E24" s="16">
+        <v>23601.691999999999</v>
+      </c>
       <c r="F24" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>6.5560255555555553</v>
+      </c>
+      <c r="G24" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="6">
+        <v>42.893900000000002</v>
+      </c>
+      <c r="E25" s="16">
+        <v>20693.037700000001</v>
+      </c>
       <c r="F25" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>5.748066027777778</v>
+      </c>
+      <c r="G25" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
       <c r="C26" s="25">
         <v>1.25</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="6">
+        <v>42.756799999999998</v>
+      </c>
+      <c r="E26" s="16">
+        <v>17522.429700000001</v>
+      </c>
       <c r="F26" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="7"/>
+        <v>4.8673415833333333</v>
+      </c>
+      <c r="G26" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="6">
+        <v>43.082599999999999</v>
+      </c>
+      <c r="E27" s="16">
+        <v>26337.511200000001</v>
+      </c>
       <c r="F27" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="7"/>
+        <v>7.3159753333333333</v>
+      </c>
+      <c r="G27" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="6">
+        <v>42.710799999999999</v>
+      </c>
+      <c r="E28" s="16">
+        <v>17947.154399999999</v>
+      </c>
       <c r="F28" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="7"/>
+        <v>4.9853206666666665</v>
+      </c>
+      <c r="G28" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="6">
+        <v>42.746400000000001</v>
+      </c>
+      <c r="E29" s="16">
+        <v>16070.111000000001</v>
+      </c>
       <c r="F29" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="7"/>
+        <v>4.4639197222222222</v>
+      </c>
+      <c r="G29" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
       <c r="C30" s="25">
         <v>1.25</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="16"/>
+      <c r="D30" s="6">
+        <v>42.915700000000001</v>
+      </c>
+      <c r="E30" s="16">
+        <v>23646.232899999999</v>
+      </c>
       <c r="F30" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="7"/>
+        <v>6.5683980277777776</v>
+      </c>
+      <c r="G30" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="16"/>
+      <c r="D31" s="6">
+        <v>42.592100000000002</v>
+      </c>
+      <c r="E31" s="16">
+        <v>18766.511200000001</v>
+      </c>
       <c r="F31" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="7"/>
+        <v>5.2129197777777776</v>
+      </c>
+      <c r="G31" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="16"/>
+      <c r="D32" s="6">
+        <v>42.393799999999999</v>
+      </c>
+      <c r="E32" s="16">
+        <v>14508.1584</v>
+      </c>
       <c r="F32" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="7"/>
+        <v>4.0300440000000002</v>
+      </c>
+      <c r="G32" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="16"/>
+      <c r="D33" s="6">
+        <v>42.602400000000003</v>
+      </c>
+      <c r="E33" s="16">
+        <v>16030.91</v>
+      </c>
       <c r="F33" s="19">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="7"/>
+        <v>4.4530305555555554</v>
+      </c>
+      <c r="G33" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3819,7 +4005,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -3837,7 +4023,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3851,7 +4037,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3865,7 +4051,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3879,7 +4065,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -3895,7 +4081,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3909,7 +4095,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3923,7 +4109,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3937,7 +4123,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -3953,7 +4139,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3967,7 +4153,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3981,7 +4167,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3995,7 +4181,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4011,7 +4197,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4025,7 +4211,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4039,7 +4225,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4056,16 +4242,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5509,12 +5695,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5747,17 +5932,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5782,18 +5977,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Finalise opus base AoN adapt wce results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2443" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95DD70C4-41FE-45B5-BAC8-3559C442D11F}"/>
+  <xr:revisionPtr revIDLastSave="2458" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D16211C-5193-4D86-BAC5-AB2C8E2E8A4B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
   <si>
     <t>Weight</t>
   </si>
@@ -114,9 +114,6 @@
   </si>
   <si>
     <t>Weighted Proportion</t>
-  </si>
-  <si>
-    <t>RERUN</t>
   </si>
 </sst>
 </file>
@@ -574,6 +571,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -583,24 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -629,39 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1008,13 +1005,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="36">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1036,9 +1033,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1058,9 +1055,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1080,9 +1077,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1102,9 +1099,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61">
+      <c r="A6" s="38"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1126,9 +1123,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1148,9 +1145,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1170,9 +1167,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1192,9 +1189,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61">
+      <c r="A10" s="38"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1216,9 +1213,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1238,9 +1235,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1260,9 +1257,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1282,9 +1279,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61">
+      <c r="A14" s="38"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1306,9 +1303,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1328,9 +1325,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1350,9 +1347,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1372,11 +1369,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="57"/>
-      <c r="B18" s="53">
+      <c r="A18" s="38"/>
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1396,9 +1393,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="57"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="61"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1418,9 +1415,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="57"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="61"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1440,9 +1437,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="61"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1462,11 +1459,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="57"/>
-      <c r="B22" s="61">
+      <c r="A22" s="38"/>
+      <c r="B22" s="44">
         <v>0.75</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1486,9 +1483,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="57"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1507,9 +1504,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="57"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1529,9 +1526,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1551,11 +1548,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="61">
+      <c r="A26" s="38"/>
+      <c r="B26" s="44">
         <v>0.5</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1575,9 +1572,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="57"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1597,9 +1594,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1619,9 +1616,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1641,11 +1638,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="61">
+      <c r="A30" s="38"/>
+      <c r="B30" s="44">
         <v>0.25</v>
       </c>
-      <c r="C30" s="61"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1665,9 +1662,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1687,9 +1684,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1709,9 +1706,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1731,13 +1728,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="46">
         <v>0.1</v>
       </c>
-      <c r="C34" s="63">
+      <c r="C34" s="46">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1759,9 +1756,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1781,9 +1778,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="39"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1803,9 +1800,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1825,14 +1822,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1849,12 +1846,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1871,13 +1868,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1899,9 +1896,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="52"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1923,11 +1920,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="46" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="47"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1949,9 +1946,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1973,14 +1970,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="36"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1997,12 +1994,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="38"/>
-      <c r="B45" s="40" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2019,12 +2016,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2051,6 +2048,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2067,13 +2071,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2486,7 +2483,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2512,7 +2509,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2534,7 +2531,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2556,7 +2553,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2578,7 +2575,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2602,7 +2599,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2623,7 +2620,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2645,7 +2642,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2667,7 +2664,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2691,7 +2688,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2713,7 +2710,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2735,7 +2732,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2757,7 +2754,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2781,7 +2778,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2803,7 +2800,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2825,7 +2822,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3021,7 +3018,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I14:I15"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3191,15 +3188,18 @@
       <c r="C8" s="23">
         <v>1.75</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="6">
+        <v>42.420200000000001</v>
+      </c>
+      <c r="E8" s="15">
+        <v>17695.0713</v>
+      </c>
       <c r="F8" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="7"/>
-      <c r="H8" s="30" t="s">
-        <v>24</v>
+        <v>4.9152975833333334</v>
+      </c>
+      <c r="G8" s="7">
+        <v>82.794399999999996</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
@@ -3208,15 +3208,18 @@
       <c r="C9" s="23">
         <v>2</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="6">
+        <v>42.545699999999997</v>
+      </c>
+      <c r="E9" s="15">
+        <v>17824.733899999999</v>
+      </c>
       <c r="F9" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="7"/>
-      <c r="H9" s="30" t="s">
-        <v>24</v>
+        <v>4.9513149722222218</v>
+      </c>
+      <c r="G9" s="7">
+        <v>82.794399999999996</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
@@ -3309,15 +3312,18 @@
       <c r="C14" s="25">
         <v>1.25</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="16"/>
+      <c r="D14" s="6">
+        <v>42.499600000000001</v>
+      </c>
+      <c r="E14" s="16">
+        <v>20941.573199999999</v>
+      </c>
       <c r="F14" s="19">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="7"/>
-      <c r="H14" s="30" t="s">
-        <v>24</v>
+        <v>5.8171036666666662</v>
+      </c>
+      <c r="G14" s="7">
+        <v>103.4885</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -3381,7 +3387,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3405,7 +3411,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3425,7 +3431,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3445,7 +3451,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3465,7 +3471,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3487,7 +3493,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3507,7 +3513,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3527,7 +3533,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3547,7 +3553,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3569,12 +3575,12 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
-      <c r="D27" s="6">
+      <c r="D27" s="12">
         <v>43.082599999999999</v>
       </c>
       <c r="E27" s="16">
@@ -3589,7 +3595,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3609,7 +3615,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3629,7 +3635,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3651,7 +3657,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3671,7 +3677,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3691,7 +3697,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3712,16 +3718,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4005,7 +4011,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -4023,7 +4029,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -4037,7 +4043,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -4051,7 +4057,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -4065,7 +4071,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -4081,7 +4087,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -4095,7 +4101,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -4109,7 +4115,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -4123,7 +4129,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -4139,7 +4145,7 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -4153,7 +4159,7 @@
       <c r="G27" s="7"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -4167,7 +4173,7 @@
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -4181,7 +4187,7 @@
       <c r="G29" s="7"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4197,7 +4203,7 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4211,7 +4217,7 @@
       <c r="G31" s="7"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4225,7 +4231,7 @@
       <c r="G32" s="7"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4242,16 +4248,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5695,11 +5701,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5932,27 +5939,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5977,9 +5974,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
File some results from opus-base fine and lsp simple wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2458" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D16211C-5193-4D86-BAC5-AB2C8E2E8A4B}"/>
+  <xr:revisionPtr revIDLastSave="2491" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7F23BEB-A226-4CBD-AECB-E3AA7BD39BAB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -571,6 +571,57 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -580,24 +631,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -626,39 +659,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,13 +1005,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="37" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="55">
+      <c r="C2" s="36">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1033,9 +1033,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="57"/>
-      <c r="B3" s="61"/>
-      <c r="C3" s="61"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="44"/>
+      <c r="C3" s="44"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1055,9 +1055,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="57"/>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="44"/>
+      <c r="C4" s="44"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1077,9 +1077,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="57"/>
-      <c r="B5" s="61"/>
-      <c r="C5" s="61"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="44"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1099,9 +1099,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="57"/>
-      <c r="B6" s="61"/>
-      <c r="C6" s="61">
+      <c r="A6" s="38"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1123,9 +1123,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="57"/>
-      <c r="B7" s="61"/>
-      <c r="C7" s="61"/>
+      <c r="A7" s="38"/>
+      <c r="B7" s="44"/>
+      <c r="C7" s="44"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1145,9 +1145,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="57"/>
-      <c r="B8" s="61"/>
-      <c r="C8" s="61"/>
+      <c r="A8" s="38"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1167,9 +1167,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="57"/>
-      <c r="B9" s="61"/>
-      <c r="C9" s="61"/>
+      <c r="A9" s="38"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1189,9 +1189,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
-      <c r="B10" s="61"/>
-      <c r="C10" s="61">
+      <c r="A10" s="38"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="44">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1213,9 +1213,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="57"/>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
+      <c r="A11" s="38"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1235,9 +1235,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="57"/>
-      <c r="B12" s="61"/>
-      <c r="C12" s="61"/>
+      <c r="A12" s="38"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1257,9 +1257,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="57"/>
-      <c r="B13" s="61"/>
-      <c r="C13" s="61"/>
+      <c r="A13" s="38"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="44"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1279,9 +1279,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="57"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61">
+      <c r="A14" s="38"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="44">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1303,9 +1303,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="57"/>
-      <c r="B15" s="61"/>
-      <c r="C15" s="61"/>
+      <c r="A15" s="38"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="44"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1325,9 +1325,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
-      <c r="B16" s="61"/>
-      <c r="C16" s="61"/>
+      <c r="A16" s="38"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="44"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1347,9 +1347,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
-      <c r="B17" s="61"/>
-      <c r="C17" s="61"/>
+      <c r="A17" s="38"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="44"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1369,11 +1369,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="57"/>
-      <c r="B18" s="53">
+      <c r="A18" s="38"/>
+      <c r="B18" s="34">
         <v>1</v>
       </c>
-      <c r="C18" s="61"/>
+      <c r="C18" s="44"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1393,9 +1393,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="57"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="61"/>
+      <c r="A19" s="38"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="44"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1415,9 +1415,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="57"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="61"/>
+      <c r="A20" s="38"/>
+      <c r="B20" s="35"/>
+      <c r="C20" s="44"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1437,9 +1437,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="57"/>
-      <c r="B21" s="55"/>
-      <c r="C21" s="61"/>
+      <c r="A21" s="38"/>
+      <c r="B21" s="36"/>
+      <c r="C21" s="44"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1459,11 +1459,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="57"/>
-      <c r="B22" s="61">
+      <c r="A22" s="38"/>
+      <c r="B22" s="44">
         <v>0.75</v>
       </c>
-      <c r="C22" s="61"/>
+      <c r="C22" s="44"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1483,9 +1483,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="57"/>
-      <c r="B23" s="61"/>
-      <c r="C23" s="61"/>
+      <c r="A23" s="38"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1504,9 +1504,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="57"/>
-      <c r="B24" s="61"/>
-      <c r="C24" s="61"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="44"/>
+      <c r="C24" s="44"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1526,9 +1526,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="57"/>
-      <c r="B25" s="61"/>
-      <c r="C25" s="61"/>
+      <c r="A25" s="38"/>
+      <c r="B25" s="44"/>
+      <c r="C25" s="44"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1548,11 +1548,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="57"/>
-      <c r="B26" s="61">
+      <c r="A26" s="38"/>
+      <c r="B26" s="44">
         <v>0.5</v>
       </c>
-      <c r="C26" s="61"/>
+      <c r="C26" s="44"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1572,9 +1572,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="57"/>
-      <c r="B27" s="61"/>
-      <c r="C27" s="61"/>
+      <c r="A27" s="38"/>
+      <c r="B27" s="44"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1594,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="57"/>
-      <c r="B28" s="61"/>
-      <c r="C28" s="61"/>
+      <c r="A28" s="38"/>
+      <c r="B28" s="44"/>
+      <c r="C28" s="44"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1616,9 +1616,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="57"/>
-      <c r="B29" s="61"/>
-      <c r="C29" s="61"/>
+      <c r="A29" s="38"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1638,11 +1638,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="57"/>
-      <c r="B30" s="61">
+      <c r="A30" s="38"/>
+      <c r="B30" s="44">
         <v>0.25</v>
       </c>
-      <c r="C30" s="61"/>
+      <c r="C30" s="44"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1662,9 +1662,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="57"/>
-      <c r="B31" s="61"/>
-      <c r="C31" s="61"/>
+      <c r="A31" s="38"/>
+      <c r="B31" s="44"/>
+      <c r="C31" s="44"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1684,9 +1684,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="57"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
+      <c r="A32" s="38"/>
+      <c r="B32" s="44"/>
+      <c r="C32" s="44"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1706,9 +1706,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="58"/>
-      <c r="B33" s="62"/>
-      <c r="C33" s="62"/>
+      <c r="A33" s="39"/>
+      <c r="B33" s="45"/>
+      <c r="C33" s="45"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1728,13 +1728,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="59" t="s">
+      <c r="A34" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="63">
+      <c r="B34" s="46">
         <v>0.1</v>
       </c>
-      <c r="C34" s="63">
+      <c r="C34" s="46">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1756,9 +1756,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="39"/>
-      <c r="B35" s="61"/>
-      <c r="C35" s="61"/>
+      <c r="A35" s="41"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1778,9 +1778,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="39"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="61"/>
+      <c r="A36" s="41"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="44"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1800,9 +1800,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="38"/>
-      <c r="B37" s="62"/>
-      <c r="C37" s="62"/>
+      <c r="A37" s="42"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1822,14 +1822,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="43" t="s">
+      <c r="B38" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="44"/>
-      <c r="D38" s="45"/>
+      <c r="C38" s="55"/>
+      <c r="D38" s="56"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1846,12 +1846,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="38"/>
-      <c r="B39" s="40" t="s">
+      <c r="A39" s="42"/>
+      <c r="B39" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="41"/>
-      <c r="D39" s="42"/>
+      <c r="C39" s="49"/>
+      <c r="D39" s="50"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1868,13 +1868,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="37" t="s">
+      <c r="A40" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="50" t="s">
+      <c r="B40" s="61" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="51"/>
+      <c r="C40" s="62"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1896,9 +1896,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="39"/>
-      <c r="B41" s="43"/>
-      <c r="C41" s="52"/>
+      <c r="A41" s="41"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="63"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1920,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="39"/>
-      <c r="B42" s="46" t="s">
+      <c r="A42" s="41"/>
+      <c r="B42" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="47"/>
+      <c r="C42" s="58"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1946,9 +1946,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="38"/>
-      <c r="B43" s="48"/>
-      <c r="C43" s="49"/>
+      <c r="A43" s="42"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="60"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1970,14 +1970,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="37" t="s">
+      <c r="A44" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="34" t="s">
+      <c r="B44" s="51" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="35"/>
-      <c r="D44" s="36"/>
+      <c r="C44" s="52"/>
+      <c r="D44" s="53"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1994,12 +1994,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="38"/>
-      <c r="B45" s="40" t="s">
+      <c r="A45" s="42"/>
+      <c r="B45" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="42"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="50"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2016,12 +2016,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="60" t="s">
+      <c r="A46" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="60"/>
-      <c r="C46" s="60"/>
-      <c r="D46" s="60"/>
+      <c r="B46" s="43"/>
+      <c r="C46" s="43"/>
+      <c r="D46" s="43"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2048,6 +2048,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2064,13 +2071,6 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2483,7 +2483,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2509,7 +2509,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2531,7 +2531,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2553,7 +2553,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2575,7 +2575,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2599,7 +2599,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2620,7 +2620,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2642,7 +2642,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2664,7 +2664,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2688,7 +2688,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2710,7 +2710,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2732,7 +2732,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2754,7 +2754,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2778,7 +2778,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2800,7 +2800,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2822,7 +2822,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3017,7 +3017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B44CA5E-D6A9-491D-9F24-D323A0E66CBD}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
@@ -3387,7 +3387,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3411,7 +3411,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3431,7 +3431,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3451,7 +3451,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3471,7 +3471,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3493,7 +3493,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3513,7 +3513,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3533,7 +3533,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3553,7 +3553,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3575,7 +3575,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3595,7 +3595,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3615,7 +3615,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3635,7 +3635,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3657,7 +3657,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3677,7 +3677,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3697,7 +3697,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3718,16 +3718,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3738,8 +3738,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4007DDC-E746-4472-AC8B-DF55C0CDCC5B}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3786,13 +3786,19 @@
       <c r="C2" s="25">
         <v>1.25</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="14"/>
+      <c r="D2" s="4">
+        <v>42.681800000000003</v>
+      </c>
+      <c r="E2" s="14">
+        <v>20897.060000000001</v>
+      </c>
       <c r="F2" s="5">
         <f>E2/3600</f>
-        <v>0</v>
-      </c>
-      <c r="G2" s="5"/>
+        <v>5.8047388888888891</v>
+      </c>
+      <c r="G2" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
@@ -3800,13 +3806,19 @@
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="15"/>
+      <c r="D3" s="6">
+        <v>42.476500000000001</v>
+      </c>
+      <c r="E3" s="15">
+        <v>18880.173999999999</v>
+      </c>
       <c r="F3" s="5">
         <f t="shared" ref="F3:F33" si="0">E3/3600</f>
-        <v>0</v>
-      </c>
-      <c r="G3" s="7"/>
+        <v>5.2444927777777774</v>
+      </c>
+      <c r="G3" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
@@ -3828,13 +3840,19 @@
       <c r="C5" s="23">
         <v>2</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="15"/>
+      <c r="D5" s="6">
+        <v>42.572200000000002</v>
+      </c>
+      <c r="E5" s="15">
+        <v>17409.0831</v>
+      </c>
       <c r="F5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G5" s="7"/>
+        <v>4.8358564166666662</v>
+      </c>
+      <c r="G5" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="65"/>
@@ -3988,13 +4006,19 @@
       <c r="C16" s="23">
         <v>1.75</v>
       </c>
-      <c r="D16" s="6"/>
-      <c r="E16" s="15"/>
+      <c r="D16" s="6">
+        <v>42.638800000000003</v>
+      </c>
+      <c r="E16" s="15">
+        <v>16184.869699999999</v>
+      </c>
       <c r="F16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G16" s="7"/>
+        <v>4.4957971388888884</v>
+      </c>
+      <c r="G16" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
@@ -4011,7 +4035,7 @@
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="53" t="s">
+      <c r="A18" s="34" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -4029,7 +4053,7 @@
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="54"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -4043,7 +4067,7 @@
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="54"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -4057,7 +4081,7 @@
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="54"/>
+      <c r="A21" s="35"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -4071,7 +4095,7 @@
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="54"/>
+      <c r="A22" s="35"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -4087,7 +4111,7 @@
       <c r="G22" s="7"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="54"/>
+      <c r="A23" s="35"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -4101,7 +4125,7 @@
       <c r="G23" s="7"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="54"/>
+      <c r="A24" s="35"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -4115,7 +4139,7 @@
       <c r="G24" s="7"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="54"/>
+      <c r="A25" s="35"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -4129,7 +4153,7 @@
       <c r="G25" s="7"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="54"/>
+      <c r="A26" s="35"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -4145,49 +4169,67 @@
       <c r="G26" s="7"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="54"/>
+      <c r="A27" s="35"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
       </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="16"/>
+      <c r="D27" s="6">
+        <v>42.6387</v>
+      </c>
+      <c r="E27" s="16">
+        <v>16033.4198</v>
+      </c>
       <c r="F27" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G27" s="7"/>
+        <v>4.4537277222222222</v>
+      </c>
+      <c r="G27" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="54"/>
+      <c r="A28" s="35"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
       </c>
-      <c r="D28" s="6"/>
-      <c r="E28" s="16"/>
+      <c r="D28" s="6">
+        <v>42.819200000000002</v>
+      </c>
+      <c r="E28" s="16">
+        <v>20605.7837</v>
+      </c>
       <c r="F28" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G28" s="7"/>
+        <v>5.7238288055555557</v>
+      </c>
+      <c r="G28" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="54"/>
+      <c r="A29" s="35"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
       </c>
-      <c r="D29" s="6"/>
-      <c r="E29" s="16"/>
+      <c r="D29" s="6">
+        <v>42.6922</v>
+      </c>
+      <c r="E29" s="16">
+        <v>17236.734499999999</v>
+      </c>
       <c r="F29" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G29" s="7"/>
+        <v>4.787981805555555</v>
+      </c>
+      <c r="G29" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="54"/>
+      <c r="A30" s="35"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4203,35 +4245,47 @@
       <c r="G30" s="7"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="54"/>
+      <c r="A31" s="35"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
       </c>
-      <c r="D31" s="6"/>
-      <c r="E31" s="16"/>
+      <c r="D31" s="6">
+        <v>42.620199999999997</v>
+      </c>
+      <c r="E31" s="16">
+        <v>17427.864399999999</v>
+      </c>
       <c r="F31" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G31" s="7"/>
+        <v>4.8410734444444437</v>
+      </c>
+      <c r="G31" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="54"/>
+      <c r="A32" s="35"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
       </c>
-      <c r="D32" s="6"/>
-      <c r="E32" s="16"/>
+      <c r="D32" s="6">
+        <v>42.666800000000002</v>
+      </c>
+      <c r="E32" s="16">
+        <v>25362.616900000001</v>
+      </c>
       <c r="F32" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G32" s="7"/>
+        <v>7.0451713611111115</v>
+      </c>
+      <c r="G32" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="55"/>
+      <c r="A33" s="36"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4248,16 +4302,16 @@
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A2:A17"/>
+    <mergeCell ref="B2:B5"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="B10:B13"/>
+    <mergeCell ref="B14:B17"/>
     <mergeCell ref="A18:A33"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="B26:B29"/>
     <mergeCell ref="B30:B33"/>
-    <mergeCell ref="A2:A17"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="B10:B13"/>
-    <mergeCell ref="B14:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4269,7 +4323,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4340,13 +4394,19 @@
       <c r="B4" s="23">
         <v>1.75</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="6">
+        <v>42.277900000000002</v>
+      </c>
+      <c r="D4" s="15">
+        <v>12264.431500000001</v>
+      </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>3.4067865277777778</v>
+      </c>
+      <c r="F4" s="7">
+        <v>89.692099999999996</v>
+      </c>
       <c r="G4" s="28"/>
       <c r="H4" s="10"/>
     </row>
@@ -4417,13 +4477,19 @@
       <c r="B9" s="23">
         <v>2</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="6">
+        <v>43.1111</v>
+      </c>
+      <c r="D9" s="15">
+        <v>23602.464199999999</v>
+      </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>6.5562400555555556</v>
+      </c>
+      <c r="F9" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G9" s="28"/>
       <c r="H9" s="10"/>
     </row>
@@ -4866,7 +4932,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E17"/>
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5284,7 +5350,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5701,11 +5767,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5938,27 +6005,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5983,9 +6040,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Add final opus-base fine adapt wce and some lsp simple results
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2491" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7F23BEB-A226-4CBD-AECB-E3AA7BD39BAB}"/>
+  <xr:revisionPtr revIDLastSave="2613" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F2C3695-EC97-4C6B-8160-2B8D18B564E1}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -2082,7 +2082,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2422,7 +2422,7 @@
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="12">
         <v>42.741199999999999</v>
       </c>
       <c r="E15" s="15">
@@ -3018,7 +3018,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3085,7 +3085,7 @@
       <c r="C3" s="23">
         <v>1.5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="12">
         <v>42.887900000000002</v>
       </c>
       <c r="E3" s="15">
@@ -3739,7 +3739,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3826,13 +3826,19 @@
       <c r="C4" s="23">
         <v>1.75</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="15"/>
+      <c r="D4" s="6">
+        <v>42.5869</v>
+      </c>
+      <c r="E4" s="15">
+        <v>19109.868900000001</v>
+      </c>
       <c r="F4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G4" s="7"/>
+        <v>5.3082969166666674</v>
+      </c>
+      <c r="G4" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="65"/>
@@ -3862,13 +3868,19 @@
       <c r="C6" s="25">
         <v>1.25</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="15"/>
+      <c r="D6" s="6">
+        <v>42.600099999999998</v>
+      </c>
+      <c r="E6" s="15">
+        <v>17395.145799999998</v>
+      </c>
       <c r="F6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
+        <v>4.8319849444444438</v>
+      </c>
+      <c r="G6" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
@@ -3876,13 +3888,19 @@
       <c r="C7" s="23">
         <v>1.5</v>
       </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="15"/>
+      <c r="D7" s="6">
+        <v>42.297699999999999</v>
+      </c>
+      <c r="E7" s="15">
+        <v>16430.728299999999</v>
+      </c>
       <c r="F7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="7"/>
+        <v>4.564091194444444</v>
+      </c>
+      <c r="G7" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
@@ -3890,13 +3908,19 @@
       <c r="C8" s="23">
         <v>1.75</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="6">
+        <v>42.670999999999999</v>
+      </c>
+      <c r="E8" s="15">
+        <v>17620.359799999998</v>
+      </c>
       <c r="F8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G8" s="7"/>
+        <v>4.8945443888888889</v>
+      </c>
+      <c r="G8" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="65"/>
@@ -3904,13 +3928,19 @@
       <c r="C9" s="23">
         <v>2</v>
       </c>
-      <c r="D9" s="6"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="6">
+        <v>42.6693</v>
+      </c>
+      <c r="E9" s="15">
+        <v>22515.164000000001</v>
+      </c>
       <c r="F9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G9" s="7"/>
+        <v>6.2542122222222227</v>
+      </c>
+      <c r="G9" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="65"/>
@@ -3920,13 +3950,19 @@
       <c r="C10" s="25">
         <v>1.25</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="6">
+        <v>42.499400000000001</v>
+      </c>
+      <c r="E10" s="15">
+        <v>17713.3151</v>
+      </c>
       <c r="F10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G10" s="7"/>
+        <v>4.9203653055555554</v>
+      </c>
+      <c r="G10" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
@@ -3934,13 +3970,19 @@
       <c r="C11" s="23">
         <v>1.5</v>
       </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="15"/>
+      <c r="D11" s="6">
+        <v>42.659300000000002</v>
+      </c>
+      <c r="E11" s="15">
+        <v>20801.682199999999</v>
+      </c>
       <c r="F11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G11" s="7"/>
+        <v>5.7782450555555558</v>
+      </c>
+      <c r="G11" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
@@ -3948,13 +3990,19 @@
       <c r="C12" s="23">
         <v>1.75</v>
       </c>
-      <c r="D12" s="6"/>
-      <c r="E12" s="15"/>
+      <c r="D12" s="6">
+        <v>42.381799999999998</v>
+      </c>
+      <c r="E12" s="15">
+        <v>17628.0972</v>
+      </c>
       <c r="F12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G12" s="7"/>
+        <v>4.8966936666666667</v>
+      </c>
+      <c r="G12" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="65"/>
@@ -3962,13 +4010,19 @@
       <c r="C13" s="23">
         <v>2</v>
       </c>
-      <c r="D13" s="6"/>
-      <c r="E13" s="15"/>
+      <c r="D13" s="6">
+        <v>42.747199999999999</v>
+      </c>
+      <c r="E13" s="15">
+        <v>17665.2372</v>
+      </c>
       <c r="F13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G13" s="7"/>
+        <v>4.907010333333333</v>
+      </c>
+      <c r="G13" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="65"/>
@@ -3978,13 +4032,19 @@
       <c r="C14" s="25">
         <v>1.25</v>
       </c>
-      <c r="D14" s="6"/>
-      <c r="E14" s="16"/>
+      <c r="D14" s="12">
+        <v>42.772199999999998</v>
+      </c>
+      <c r="E14" s="16">
+        <v>22714.4349</v>
+      </c>
       <c r="F14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G14" s="7"/>
+        <v>6.3095652500000003</v>
+      </c>
+      <c r="G14" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="65"/>
@@ -3992,13 +4052,19 @@
       <c r="C15" s="23">
         <v>1.5</v>
       </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="15"/>
+      <c r="D15" s="6">
+        <v>42.045999999999999</v>
+      </c>
+      <c r="E15" s="15">
+        <v>10507.374400000001</v>
+      </c>
       <c r="F15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G15" s="7"/>
+        <v>2.9187151111111111</v>
+      </c>
+      <c r="G15" s="7">
+        <v>69.000799999999998</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
@@ -4026,13 +4092,19 @@
       <c r="C17" s="23">
         <v>2</v>
       </c>
-      <c r="D17" s="6"/>
-      <c r="E17" s="16"/>
+      <c r="D17" s="6">
+        <v>42.594099999999997</v>
+      </c>
+      <c r="E17" s="16">
+        <v>20454.816200000001</v>
+      </c>
       <c r="F17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G17" s="7"/>
+        <v>5.6818933888888896</v>
+      </c>
+      <c r="G17" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="34" t="s">
@@ -4044,13 +4116,19 @@
       <c r="C18" s="25">
         <v>1.25</v>
       </c>
-      <c r="D18" s="6"/>
-      <c r="E18" s="16"/>
+      <c r="D18" s="6">
+        <v>42.690899999999999</v>
+      </c>
+      <c r="E18" s="16">
+        <v>20444.894700000001</v>
+      </c>
       <c r="F18" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G18" s="7"/>
+        <v>5.6791374166666673</v>
+      </c>
+      <c r="G18" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="35"/>
@@ -4058,13 +4136,19 @@
       <c r="C19" s="23">
         <v>1.5</v>
       </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="16"/>
+      <c r="D19" s="6">
+        <v>42.612000000000002</v>
+      </c>
+      <c r="E19" s="16">
+        <v>18350.4892</v>
+      </c>
       <c r="F19" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G19" s="7"/>
+        <v>5.0973581111111113</v>
+      </c>
+      <c r="G19" s="7">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="35"/>
@@ -4072,13 +4156,19 @@
       <c r="C20" s="23">
         <v>1.75</v>
       </c>
-      <c r="D20" s="6"/>
-      <c r="E20" s="16"/>
+      <c r="D20" s="6">
+        <v>42.553800000000003</v>
+      </c>
+      <c r="E20" s="16">
+        <v>14190.751399999999</v>
+      </c>
       <c r="F20" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G20" s="7"/>
+        <v>3.9418753888888887</v>
+      </c>
+      <c r="G20" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="35"/>
@@ -4086,13 +4176,19 @@
       <c r="C21" s="23">
         <v>2</v>
       </c>
-      <c r="D21" s="6"/>
-      <c r="E21" s="16"/>
+      <c r="D21" s="6">
+        <v>42.829099999999997</v>
+      </c>
+      <c r="E21" s="16">
+        <v>22787.285</v>
+      </c>
       <c r="F21" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G21" s="7"/>
+        <v>6.3298013888888889</v>
+      </c>
+      <c r="G21" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="35"/>
@@ -4102,13 +4198,19 @@
       <c r="C22" s="25">
         <v>1.25</v>
       </c>
-      <c r="D22" s="6"/>
-      <c r="E22" s="16"/>
+      <c r="D22" s="6">
+        <v>42.479799999999997</v>
+      </c>
+      <c r="E22" s="16">
+        <v>15149.1173</v>
+      </c>
       <c r="F22" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G22" s="7"/>
+        <v>4.2080881388888889</v>
+      </c>
+      <c r="G22" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="35"/>
@@ -4116,13 +4218,19 @@
       <c r="C23" s="23">
         <v>1.5</v>
       </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="16"/>
+      <c r="D23" s="6">
+        <v>42.753100000000003</v>
+      </c>
+      <c r="E23" s="16">
+        <v>16079.589599999999</v>
+      </c>
       <c r="F23" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>4.4665526666666668</v>
+      </c>
+      <c r="G23" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="35"/>
@@ -4130,13 +4238,19 @@
       <c r="C24" s="23">
         <v>1.75</v>
       </c>
-      <c r="D24" s="6"/>
-      <c r="E24" s="16"/>
+      <c r="D24" s="6">
+        <v>42.702199999999998</v>
+      </c>
+      <c r="E24" s="16">
+        <v>20685.9015</v>
+      </c>
       <c r="F24" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>5.7460837500000004</v>
+      </c>
+      <c r="G24" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="35"/>
@@ -4144,13 +4258,19 @@
       <c r="C25" s="23">
         <v>2</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="16"/>
+      <c r="D25" s="6">
+        <v>42.891399999999997</v>
+      </c>
+      <c r="E25" s="16">
+        <v>25843.4002</v>
+      </c>
       <c r="F25" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>7.1787222777777782</v>
+      </c>
+      <c r="G25" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="35"/>
@@ -4160,13 +4280,19 @@
       <c r="C26" s="25">
         <v>1.25</v>
       </c>
-      <c r="D26" s="6"/>
-      <c r="E26" s="16"/>
+      <c r="D26" s="6">
+        <v>42.534399999999998</v>
+      </c>
+      <c r="E26" s="16">
+        <v>16114.2562</v>
+      </c>
       <c r="F26" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G26" s="7"/>
+        <v>4.4761822777777773</v>
+      </c>
+      <c r="G26" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="35"/>
@@ -4236,13 +4362,19 @@
       <c r="C30" s="25">
         <v>1.25</v>
       </c>
-      <c r="D30" s="6"/>
-      <c r="E30" s="16"/>
+      <c r="D30" s="6">
+        <v>42.553899999999999</v>
+      </c>
+      <c r="E30" s="16">
+        <v>16043.049000000001</v>
+      </c>
       <c r="F30" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G30" s="7"/>
+        <v>4.4564025000000003</v>
+      </c>
+      <c r="G30" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="35"/>
@@ -4290,13 +4422,19 @@
       <c r="C33" s="23">
         <v>2</v>
       </c>
-      <c r="D33" s="6"/>
-      <c r="E33" s="16"/>
+      <c r="D33" s="12">
+        <v>42.909500000000001</v>
+      </c>
+      <c r="E33" s="16">
+        <v>25622.4293</v>
+      </c>
       <c r="F33" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G33" s="7"/>
+        <v>7.1173414722222219</v>
+      </c>
+      <c r="G33" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4323,7 +4461,7 @@
   <dimension ref="A1:H47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4364,13 +4502,19 @@
       <c r="B2" s="25">
         <v>1.25</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="4">
+        <v>42.409100000000002</v>
+      </c>
+      <c r="D2" s="14">
+        <v>15410.118399999999</v>
+      </c>
       <c r="E2" s="5">
         <f>D2/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>4.2805884444444446</v>
+      </c>
+      <c r="F2" s="5">
+        <v>82.794399999999996</v>
+      </c>
       <c r="G2" s="28"/>
       <c r="H2" s="10"/>
     </row>
@@ -4379,13 +4523,19 @@
       <c r="B3" s="23">
         <v>1.5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="6">
+        <v>42.9313</v>
+      </c>
+      <c r="D3" s="15">
+        <v>23419.246299999999</v>
+      </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E17" si="0">D3/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>6.505346194444444</v>
+      </c>
+      <c r="F3" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G3" s="28"/>
       <c r="H3" s="10"/>
     </row>
@@ -4415,13 +4565,19 @@
       <c r="B5" s="23">
         <v>2</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="15"/>
+      <c r="C5" s="6">
+        <v>42.810600000000001</v>
+      </c>
+      <c r="D5" s="15">
+        <v>25720.1014</v>
+      </c>
       <c r="E5" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F5" s="7"/>
+        <v>7.1444726111111114</v>
+      </c>
+      <c r="F5" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G5" s="28"/>
       <c r="H5" s="10"/>
     </row>
@@ -4432,13 +4588,19 @@
       <c r="B6" s="25">
         <v>1.25</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="6">
+        <v>42.537199999999999</v>
+      </c>
+      <c r="D6" s="15">
+        <v>15398.700500000001</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7"/>
+        <v>4.2774168055555561</v>
+      </c>
+      <c r="F6" s="7">
+        <v>103.4885</v>
+      </c>
       <c r="G6" s="28"/>
       <c r="H6" s="10"/>
     </row>
@@ -4447,13 +4609,19 @@
       <c r="B7" s="23">
         <v>1.5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="6">
+        <v>42.713000000000001</v>
+      </c>
+      <c r="D7" s="15">
+        <v>17855.449400000001</v>
+      </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>4.9598470555555556</v>
+      </c>
+      <c r="F7" s="5">
+        <v>82.794399999999996</v>
+      </c>
       <c r="G7" s="28"/>
       <c r="H7" s="10"/>
     </row>
@@ -4462,13 +4630,19 @@
       <c r="B8" s="23">
         <v>1.75</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="6">
+        <v>42.569499999999998</v>
+      </c>
+      <c r="D8" s="15">
+        <v>17683.5304</v>
+      </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>4.9120917777777775</v>
+      </c>
+      <c r="F8" s="5">
+        <v>82.794399999999996</v>
+      </c>
       <c r="G8" s="28"/>
       <c r="H8" s="10"/>
     </row>
@@ -4500,13 +4674,19 @@
       <c r="B10" s="25">
         <v>1.25</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="6">
+        <v>42.671300000000002</v>
+      </c>
+      <c r="D10" s="15">
+        <v>18727.5838</v>
+      </c>
       <c r="E10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>5.2021066111111116</v>
+      </c>
+      <c r="F10" s="7">
+        <v>117.2388</v>
+      </c>
       <c r="G10" s="28"/>
       <c r="H10" s="10"/>
     </row>
@@ -4515,13 +4695,19 @@
       <c r="B11" s="23">
         <v>1.5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="6">
+        <v>42.667700000000004</v>
+      </c>
+      <c r="D11" s="15">
+        <v>14459.339</v>
+      </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>4.0164830555555557</v>
+      </c>
+      <c r="F11" s="7">
+        <v>103.4885</v>
+      </c>
       <c r="G11" s="28"/>
       <c r="H11" s="10"/>
     </row>
@@ -4545,13 +4731,19 @@
       <c r="B13" s="23">
         <v>2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="6">
+        <v>42.542999999999999</v>
+      </c>
+      <c r="D13" s="15">
+        <v>20668.981299999999</v>
+      </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>5.7413836944444441</v>
+      </c>
+      <c r="F13" s="7">
+        <v>103.4885</v>
+      </c>
       <c r="G13" s="28"/>
       <c r="H13" s="10"/>
     </row>
@@ -4562,13 +4754,19 @@
       <c r="B14" s="25">
         <v>1.25</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="6">
+        <v>42.842300000000002</v>
+      </c>
+      <c r="D14" s="16">
+        <v>25939.740300000001</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>7.2054834166666666</v>
+      </c>
+      <c r="F14" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G14" s="28"/>
       <c r="H14" s="10"/>
     </row>
@@ -4577,13 +4775,19 @@
       <c r="B15" s="23">
         <v>1.5</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="15"/>
+      <c r="C15" s="6">
+        <v>42.505800000000001</v>
+      </c>
+      <c r="D15" s="15">
+        <v>15643.267</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>4.3453519444444444</v>
+      </c>
+      <c r="F15" s="7">
+        <v>69.000799999999998</v>
+      </c>
       <c r="G15" s="28"/>
       <c r="H15" s="10"/>
     </row>
@@ -4592,13 +4796,19 @@
       <c r="B16" s="23">
         <v>1.75</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="15"/>
+      <c r="C16" s="6">
+        <v>42.415199999999999</v>
+      </c>
+      <c r="D16" s="15">
+        <v>14178.332700000001</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>3.9384257500000004</v>
+      </c>
+      <c r="F16" s="7">
+        <v>103.4885</v>
+      </c>
       <c r="G16" s="28"/>
       <c r="H16" s="10"/>
     </row>
@@ -4607,13 +4817,19 @@
       <c r="B17" s="23">
         <v>2</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="6">
+        <v>42.814799999999998</v>
+      </c>
+      <c r="D17" s="16">
+        <v>25285.619900000002</v>
+      </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>7.0237833055555559</v>
+      </c>
+      <c r="F17" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G17" s="28"/>
       <c r="H17" s="10"/>
     </row>

</xml_diff>

<commit_message>
Update opus-big fine adapt wce and opus-base simple lsp wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2613" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F2C3695-EC97-4C6B-8160-2B8D18B564E1}"/>
+  <xr:revisionPtr revIDLastSave="2621" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4F105B-6751-464A-841F-E55AEFCEAF54}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="25">
   <si>
     <t>Weight</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Weighted Proportion</t>
+  </si>
+  <si>
+    <t>Loaded</t>
   </si>
 </sst>
 </file>
@@ -571,6 +574,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -592,12 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -608,57 +662,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1005,13 +1008,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1033,9 +1036,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1055,9 +1058,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1077,9 +1080,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1099,9 +1102,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44">
+      <c r="A6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1123,9 +1126,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1145,9 +1148,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1167,9 +1170,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1189,9 +1192,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1213,9 +1216,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1235,9 +1238,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1257,9 +1260,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1279,9 +1282,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44">
+      <c r="A14" s="57"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1303,9 +1306,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1325,9 +1328,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1347,9 +1350,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1369,11 +1372,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="34">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1393,9 +1396,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1415,9 +1418,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1437,9 +1440,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1459,11 +1462,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44">
+      <c r="A22" s="57"/>
+      <c r="B22" s="61">
         <v>0.75</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1483,9 +1486,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1504,9 +1507,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1526,9 +1529,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1548,11 +1551,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61">
         <v>0.5</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1572,9 +1575,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1594,9 +1597,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1616,9 +1619,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1638,11 +1641,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="44">
+      <c r="A30" s="57"/>
+      <c r="B30" s="61">
         <v>0.25</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1662,9 +1665,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1684,9 +1687,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1706,9 +1709,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1728,13 +1731,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="63">
         <v>0.1</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="63">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1756,9 +1759,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1778,9 +1781,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1800,9 +1803,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1822,14 +1825,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1846,12 +1849,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="48" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1868,13 +1871,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1896,9 +1899,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1920,11 +1923,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1946,9 +1949,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1970,14 +1973,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1994,12 +1997,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="48" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2016,12 +2019,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2048,13 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2071,6 +2067,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2082,7 +2085,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2483,7 +2486,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2509,7 +2512,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2531,7 +2534,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2553,7 +2556,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2575,7 +2578,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2595,11 +2598,13 @@
       <c r="G22" s="7">
         <v>137.96010000000001</v>
       </c>
-      <c r="H22" s="28"/>
+      <c r="H22" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2620,7 +2625,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2642,7 +2647,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2664,7 +2669,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2688,7 +2693,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2710,7 +2715,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2732,7 +2737,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2754,7 +2759,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2778,7 +2783,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2800,7 +2805,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2822,7 +2827,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3018,7 +3023,7 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3366,7 +3371,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
       <c r="B17" s="68"/>
       <c r="C17" s="23">
@@ -3386,8 +3391,8 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3410,8 +3415,8 @@
         <v>117.2388</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="54"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3430,8 +3435,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="54"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3450,8 +3455,8 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="54"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3470,8 +3475,8 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="54"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3492,8 +3497,8 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="54"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3512,8 +3517,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" s="54"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3532,8 +3537,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" s="54"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3552,8 +3557,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" s="54"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3574,8 +3579,8 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" s="54"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3593,9 +3598,12 @@
       <c r="G27" s="7">
         <v>137.96010000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="H27" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" s="54"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3614,8 +3622,8 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" s="54"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3634,8 +3642,8 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" s="54"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3656,8 +3664,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" s="54"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3676,8 +3684,8 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" s="54"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3697,7 +3705,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3718,16 +3726,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -3736,10 +3744,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4007DDC-E746-4472-AC8B-DF55C0CDCC5B}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4107,7 +4115,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -4131,7 +4139,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -4151,7 +4159,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -4171,7 +4179,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -4191,7 +4199,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -4213,7 +4221,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -4233,7 +4241,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -4253,7 +4261,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -4273,7 +4281,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -4295,7 +4303,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -4315,7 +4323,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -4335,7 +4343,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -4355,7 +4363,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4377,7 +4385,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4397,7 +4405,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4416,8 +4424,8 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4435,21 +4443,24 @@
       <c r="G33" s="7">
         <v>137.96010000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:7" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="H33" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4460,8 +4471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0336D01B-C2AB-46DC-B402-9DC3749D2666}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4651,7 +4662,7 @@
       <c r="B9" s="23">
         <v>2</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="12">
         <v>43.1111</v>
       </c>
       <c r="D9" s="15">
@@ -4664,7 +4675,9 @@
       <c r="F9" s="7">
         <v>137.96010000000001</v>
       </c>
-      <c r="G9" s="28"/>
+      <c r="G9" s="28" t="s">
+        <v>24</v>
+      </c>
       <c r="H9" s="10"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -4716,13 +4729,19 @@
       <c r="B12" s="23">
         <v>1.75</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="6">
+        <v>42.839100000000002</v>
+      </c>
+      <c r="D12" s="15">
+        <v>25571.447800000002</v>
+      </c>
       <c r="E12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="5"/>
+        <v>7.1031799444444452</v>
+      </c>
+      <c r="F12" s="7">
+        <v>137.96010000000001</v>
+      </c>
       <c r="G12" s="28"/>
       <c r="H12" s="10"/>
     </row>
@@ -5983,12 +6002,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6221,17 +6239,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6256,18 +6284,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update partial results for opus-base and opus-big lsp adapt wce
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2621" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2F4F105B-6751-464A-841F-E55AEFCEAF54}"/>
+  <xr:revisionPtr revIDLastSave="2676" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7C62E228-889C-47BE-91C5-43D7432391F4}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -4471,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0336D01B-C2AB-46DC-B402-9DC3749D2666}">
   <dimension ref="A1:H47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
@@ -5167,7 +5167,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5233,13 +5233,19 @@
       <c r="B4" s="23">
         <v>1.75</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="6">
+        <v>42.412100000000002</v>
+      </c>
+      <c r="D4" s="15">
+        <v>15696.5767</v>
+      </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>4.3601601944444441</v>
+      </c>
+      <c r="F4" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="66"/>
@@ -5274,13 +5280,19 @@
       <c r="B7" s="23">
         <v>1.5</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="15"/>
+      <c r="C7" s="6">
+        <v>42.708100000000002</v>
+      </c>
+      <c r="D7" s="15">
+        <v>20739.564200000001</v>
+      </c>
       <c r="E7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>5.7609900555555553</v>
+      </c>
+      <c r="F7" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
@@ -5341,26 +5353,38 @@
       <c r="B12" s="23">
         <v>1.75</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="6">
+        <v>42.535699999999999</v>
+      </c>
+      <c r="D12" s="15">
+        <v>16222.369500000001</v>
+      </c>
       <c r="E12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>4.5062137500000006</v>
+      </c>
+      <c r="F12" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="6">
+        <v>42.737699999999997</v>
+      </c>
+      <c r="D13" s="15">
+        <v>25258.608100000001</v>
+      </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>7.0162800277777784</v>
+      </c>
+      <c r="F13" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="68">
@@ -5369,13 +5393,19 @@
       <c r="B14" s="25">
         <v>1.25</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="6">
+        <v>42.619</v>
+      </c>
+      <c r="D14" s="16">
+        <v>16232.9617</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="7"/>
+        <v>4.5091560277777774</v>
+      </c>
+      <c r="F14" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="68"/>
@@ -5584,8 +5614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBEC7E3C-257D-4C00-940F-B3A10CBB9AD7}">
   <dimension ref="A1:G47"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5625,39 +5655,57 @@
       <c r="B2" s="25">
         <v>1.25</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="14"/>
+      <c r="C2" s="4">
+        <v>42.723999999999997</v>
+      </c>
+      <c r="D2" s="14">
+        <v>22344.925999999999</v>
+      </c>
       <c r="E2" s="5">
         <f>D2/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F2" s="5"/>
+        <v>6.2069238888888885</v>
+      </c>
+      <c r="F2" s="5">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
       <c r="B3" s="23">
         <v>1.5</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="15"/>
+      <c r="C3" s="6">
+        <v>42.478099999999998</v>
+      </c>
+      <c r="D3" s="15">
+        <v>15192.597900000001</v>
+      </c>
       <c r="E3" s="5">
         <f t="shared" ref="E3:E17" si="0">D3/3600</f>
-        <v>0</v>
-      </c>
-      <c r="F3" s="7"/>
+        <v>4.2201660833333339</v>
+      </c>
+      <c r="F3" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
       <c r="B4" s="23">
         <v>1.75</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="15"/>
+      <c r="C4" s="6">
+        <v>42.533299999999997</v>
+      </c>
+      <c r="D4" s="15">
+        <v>24009.408200000002</v>
+      </c>
       <c r="E4" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F4" s="7"/>
+        <v>6.6692800555555563</v>
+      </c>
+      <c r="F4" s="7">
+        <v>131.08879999999999</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="66"/>
@@ -5705,26 +5753,38 @@
       <c r="B8" s="23">
         <v>1.75</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="6">
+        <v>42.512900000000002</v>
+      </c>
+      <c r="D8" s="15">
+        <v>24439.2444</v>
+      </c>
       <c r="E8" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>6.7886790000000001</v>
+      </c>
+      <c r="F8" s="7">
+        <v>131.08879999999999</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="66"/>
       <c r="B9" s="23">
         <v>2</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="15"/>
+      <c r="C9" s="6">
+        <v>42.6265</v>
+      </c>
+      <c r="D9" s="15">
+        <v>25073.149000000001</v>
+      </c>
       <c r="E9" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>6.9647636111111115</v>
+      </c>
+      <c r="F9" s="7">
+        <v>137.96010000000001</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="67">
@@ -5733,52 +5793,76 @@
       <c r="B10" s="25">
         <v>1.25</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="6">
+        <v>42.564599999999999</v>
+      </c>
+      <c r="D10" s="15">
+        <v>15594.134599999999</v>
+      </c>
       <c r="E10" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="7"/>
+        <v>4.331704055555555</v>
+      </c>
+      <c r="F10" s="7">
+        <v>103.4885</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
       <c r="B11" s="23">
         <v>1.5</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="15"/>
+      <c r="C11" s="6">
+        <v>42.601399999999998</v>
+      </c>
+      <c r="D11" s="15">
+        <v>17374.802299999999</v>
+      </c>
       <c r="E11" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="7"/>
+        <v>4.8263339722222218</v>
+      </c>
+      <c r="F11" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
       <c r="B12" s="23">
         <v>1.75</v>
       </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="6">
+        <v>42.185899999999997</v>
+      </c>
+      <c r="D12" s="15">
+        <v>12294.0918</v>
+      </c>
       <c r="E12" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12" s="7"/>
+        <v>3.4150255</v>
+      </c>
+      <c r="F12" s="7">
+        <v>69.000799999999998</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
       </c>
-      <c r="C13" s="6"/>
-      <c r="D13" s="15"/>
+      <c r="C13" s="6">
+        <v>42.229100000000003</v>
+      </c>
+      <c r="D13" s="15">
+        <v>14271.8639</v>
+      </c>
       <c r="E13" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F13" s="7"/>
+        <v>3.9644066388888888</v>
+      </c>
+      <c r="F13" s="7">
+        <v>69.000799999999998</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="67">
@@ -5800,39 +5884,57 @@
       <c r="B15" s="23">
         <v>1.5</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="15"/>
+      <c r="C15" s="6">
+        <v>42.681699999999999</v>
+      </c>
+      <c r="D15" s="15">
+        <v>16330.540800000001</v>
+      </c>
       <c r="E15" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="7"/>
+        <v>4.5362613333333339</v>
+      </c>
+      <c r="F15" s="7">
+        <v>82.794399999999996</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
       <c r="B16" s="23">
         <v>1.75</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="15"/>
+      <c r="C16" s="6">
+        <v>42.534700000000001</v>
+      </c>
+      <c r="D16" s="15">
+        <v>15844.378199999999</v>
+      </c>
       <c r="E16" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="7"/>
+        <v>4.401216166666666</v>
+      </c>
+      <c r="F16" s="5">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="66"/>
       <c r="B17" s="23">
         <v>2</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="16"/>
+      <c r="C17" s="6">
+        <v>42.501300000000001</v>
+      </c>
+      <c r="D17" s="16">
+        <v>17179.171600000001</v>
+      </c>
       <c r="E17" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="7"/>
+        <v>4.7719921111111114</v>
+      </c>
+      <c r="F17" s="5">
+        <v>117.2388</v>
+      </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="33"/>
@@ -6002,14 +6104,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100FED9EBA27497914FBC51691506A72748" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8db1a03e1afeb6e2a80b24d758973afd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xmlns:ns4="1a03cb65-d35a-4d70-82d7-cdf046b799c1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dd4cfb9390361c575275bc1f8c982e1d" ns3:_="" ns4:_="">
     <xsd:import namespace="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
@@ -6238,7 +6332,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -6247,24 +6341,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11A1E62E-0774-44F1-9C84-E26E87EB904E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6283,10 +6368,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Update final results from all hyp searches
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://imperiallondon-my.sharepoint.com/personal/ers19_ic_ac_uk/Documents/MSc Computing/Individual Project/Code/medical-mt/model_evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2718" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4AF586E-461E-4FB0-B60A-E4BD6EDB3898}"/>
+  <xr:revisionPtr revIDLastSave="2732" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E0E9A74-E14F-4217-B70E-A325DB83C4CF}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="25">
   <si>
     <t>Weight</t>
   </si>
@@ -574,6 +574,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -595,12 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,57 +662,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1008,13 +1008,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1036,9 +1036,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1058,9 +1058,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1080,9 +1080,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1102,9 +1102,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44">
+      <c r="A6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1126,9 +1126,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1148,9 +1148,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1170,9 +1170,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1192,9 +1192,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1216,9 +1216,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1238,9 +1238,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1260,9 +1260,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1282,9 +1282,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44">
+      <c r="A14" s="57"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1306,9 +1306,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1328,9 +1328,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1350,9 +1350,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1372,11 +1372,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="34">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1396,9 +1396,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1418,9 +1418,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1440,9 +1440,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1462,11 +1462,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44">
+      <c r="A22" s="57"/>
+      <c r="B22" s="61">
         <v>0.75</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1486,9 +1486,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1507,9 +1507,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1529,9 +1529,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1551,11 +1551,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61">
         <v>0.5</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1575,9 +1575,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1597,9 +1597,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1619,9 +1619,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1641,11 +1641,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="44">
+      <c r="A30" s="57"/>
+      <c r="B30" s="61">
         <v>0.25</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1665,9 +1665,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1687,9 +1687,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1709,9 +1709,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1731,13 +1731,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="63">
         <v>0.1</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="63">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1759,9 +1759,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1781,9 +1781,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1803,9 +1803,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1825,14 +1825,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1849,12 +1849,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="48" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1871,13 +1871,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1899,9 +1899,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1923,11 +1923,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1949,9 +1949,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1973,14 +1973,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1997,12 +1997,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="48" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2019,12 +2019,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2051,13 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2074,6 +2067,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2488,7 +2488,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2514,7 +2514,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2536,7 +2536,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2558,7 +2558,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2580,7 +2580,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2627,7 +2627,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2649,7 +2649,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2671,7 +2671,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2717,7 +2717,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2739,7 +2739,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2761,7 +2761,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2807,7 +2807,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2829,7 +2829,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3397,7 +3397,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3421,7 +3421,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3441,7 +3441,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3461,7 +3461,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3481,7 +3481,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3503,7 +3503,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3523,7 +3523,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3543,7 +3543,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3563,7 +3563,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3585,7 +3585,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3628,7 +3628,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3648,7 +3648,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3690,7 +3690,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3710,7 +3710,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3731,16 +3731,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4123,7 +4123,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -4147,7 +4147,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -4167,7 +4167,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -4207,7 +4207,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -4229,7 +4229,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -4249,7 +4249,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -4269,7 +4269,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -4289,7 +4289,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -4331,7 +4331,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -4351,7 +4351,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -4371,7 +4371,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4413,7 +4413,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4433,7 +4433,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4459,16 +4459,16 @@
     <row r="47" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5172,10 +5172,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71968B89-5396-4DBB-9374-8D1D5CD3665B}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5188,7 +5188,7 @@
     <col min="9" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>23</v>
       </c>
@@ -5208,7 +5208,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="64">
         <v>0.2</v>
       </c>
@@ -5229,7 +5229,7 @@
         <v>69.000799999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
       <c r="B3" s="23">
         <v>1.5</v>
@@ -5248,7 +5248,7 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
       <c r="B4" s="23">
         <v>1.75</v>
@@ -5267,7 +5267,7 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="66"/>
       <c r="B5" s="23">
         <v>2</v>
@@ -5286,22 +5286,31 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="67">
         <v>0.4</v>
       </c>
       <c r="B6" s="25">
         <v>1.25</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="12">
+        <v>42.747900000000001</v>
+      </c>
+      <c r="D6" s="15">
+        <v>25253.252</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>7.0147922222222228</v>
+      </c>
+      <c r="F6" s="7">
+        <v>137.96010000000001</v>
+      </c>
+      <c r="G6" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
       <c r="B7" s="23">
         <v>1.5</v>
@@ -5320,7 +5329,7 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
       <c r="B8" s="23">
         <v>1.75</v>
@@ -5339,7 +5348,7 @@
         <v>117.2388</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="66"/>
       <c r="B9" s="23">
         <v>2</v>
@@ -5358,7 +5367,7 @@
         <v>117.2388</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="67">
         <v>0.6</v>
       </c>
@@ -5379,7 +5388,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
       <c r="B11" s="23">
         <v>1.5</v>
@@ -5398,7 +5407,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
       <c r="B12" s="23">
         <v>1.75</v>
@@ -5417,7 +5426,7 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
@@ -5436,7 +5445,7 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="68">
         <v>0.8</v>
       </c>
@@ -5457,7 +5466,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="68"/>
       <c r="B15" s="23">
         <v>1.5</v>
@@ -5476,7 +5485,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="68"/>
       <c r="B16" s="23">
         <v>1.75</v>
@@ -5683,7 +5692,7 @@
   <dimension ref="A1:G47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5696,7 +5705,7 @@
     <col min="9" max="16384" width="8.88671875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>22</v>
       </c>
@@ -5716,7 +5725,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="64">
         <v>0</v>
       </c>
@@ -5737,7 +5746,7 @@
         <v>117.2388</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="65"/>
       <c r="B3" s="23">
         <v>1.5</v>
@@ -5756,7 +5765,7 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="65"/>
       <c r="B4" s="23">
         <v>1.75</v>
@@ -5775,7 +5784,7 @@
         <v>131.08879999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="66"/>
       <c r="B5" s="23">
         <v>2</v>
@@ -5794,7 +5803,7 @@
         <v>131.08879999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="67">
         <v>1</v>
       </c>
@@ -5815,12 +5824,12 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="65"/>
       <c r="B7" s="23">
         <v>1.5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="12">
         <v>42.8215</v>
       </c>
       <c r="D7" s="15">
@@ -5833,8 +5842,11 @@
       <c r="F7" s="7">
         <v>137.96010000000001</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G7" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="65"/>
       <c r="B8" s="23">
         <v>1.75</v>
@@ -5853,7 +5865,7 @@
         <v>131.08879999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="66"/>
       <c r="B9" s="23">
         <v>2</v>
@@ -5872,7 +5884,7 @@
         <v>137.96010000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="67">
         <v>2</v>
       </c>
@@ -5893,7 +5905,7 @@
         <v>103.4885</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="65"/>
       <c r="B11" s="23">
         <v>1.5</v>
@@ -5912,7 +5924,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="65"/>
       <c r="B12" s="23">
         <v>1.75</v>
@@ -5931,7 +5943,7 @@
         <v>69.000799999999998</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="66"/>
       <c r="B13" s="23">
         <v>2</v>
@@ -5950,22 +5962,28 @@
         <v>69.000799999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="67">
         <v>3</v>
       </c>
       <c r="B14" s="25">
         <v>1.25</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="16"/>
+      <c r="C14" s="6">
+        <v>42.510100000000001</v>
+      </c>
+      <c r="D14" s="16">
+        <v>15288.4319</v>
+      </c>
       <c r="E14" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F14" s="7"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+        <v>4.2467866388888886</v>
+      </c>
+      <c r="F14" s="7">
+        <v>69.000799999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="65"/>
       <c r="B15" s="23">
         <v>1.5</v>
@@ -5984,7 +6002,7 @@
         <v>82.794399999999996</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="65"/>
       <c r="B16" s="23">
         <v>1.75</v>
@@ -6190,12 +6208,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6428,17 +6445,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6463,18 +6490,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Generate simple summary statistics
</commit_message>
<xml_diff>
--- a/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
+++ b/model_evaluations/Opus-Base Hyperparameter Search Results.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="2732" documentId="8_{026E2CEC-91DE-48F7-861E-52387E5F0660}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3E0E9A74-E14F-4217-B70E-A325DB83C4CF}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="878" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="opus_base Validation " sheetId="1" r:id="rId1"/>
@@ -574,6 +574,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -595,12 +652,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -611,57 +662,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1008,13 +1008,13 @@
       <c r="I1" s="10"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="55" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="36">
+      <c r="C2" s="55">
         <v>0.25</v>
       </c>
       <c r="D2" s="4">
@@ -1036,9 +1036,9 @@
       <c r="I2" s="10"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="38"/>
-      <c r="B3" s="44"/>
-      <c r="C3" s="44"/>
+      <c r="A3" s="57"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="61"/>
       <c r="D3" s="6">
         <v>1.5</v>
       </c>
@@ -1058,9 +1058,9 @@
       <c r="I3" s="10"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="38"/>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
+      <c r="A4" s="57"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="61"/>
       <c r="D4" s="6">
         <v>1.75</v>
       </c>
@@ -1080,9 +1080,9 @@
       <c r="I4" s="10"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="38"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="44"/>
+      <c r="A5" s="57"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="61"/>
       <c r="D5" s="6">
         <v>2</v>
       </c>
@@ -1102,9 +1102,9 @@
       <c r="I5" s="10"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="38"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44">
+      <c r="A6" s="57"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61">
         <v>0.5</v>
       </c>
       <c r="D6" s="6">
@@ -1126,9 +1126,9 @@
       <c r="I6" s="10"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="38"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="A7" s="57"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="61"/>
       <c r="D7" s="6">
         <v>1.5</v>
       </c>
@@ -1148,9 +1148,9 @@
       <c r="I7" s="10"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="38"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="A8" s="57"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="61"/>
       <c r="D8" s="6">
         <v>1.75</v>
       </c>
@@ -1170,9 +1170,9 @@
       <c r="I8" s="10"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="38"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="A9" s="57"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="61"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1192,9 +1192,9 @@
       <c r="I9" s="10"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="38"/>
-      <c r="B10" s="44"/>
-      <c r="C10" s="44">
+      <c r="A10" s="57"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61">
         <v>0.75</v>
       </c>
       <c r="D10" s="6">
@@ -1216,9 +1216,9 @@
       <c r="I10" s="10"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="38"/>
-      <c r="B11" s="44"/>
-      <c r="C11" s="44"/>
+      <c r="A11" s="57"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="61"/>
       <c r="D11" s="6">
         <v>1.5</v>
       </c>
@@ -1238,9 +1238,9 @@
       <c r="I11" s="10"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="38"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
+      <c r="A12" s="57"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
       <c r="D12" s="6">
         <v>1.75</v>
       </c>
@@ -1260,9 +1260,9 @@
       <c r="I12" s="10"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="38"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
+      <c r="A13" s="57"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="6">
         <v>2</v>
       </c>
@@ -1282,9 +1282,9 @@
       <c r="I13" s="10"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="38"/>
-      <c r="B14" s="44"/>
-      <c r="C14" s="44">
+      <c r="A14" s="57"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61">
         <v>1</v>
       </c>
       <c r="D14" s="6">
@@ -1306,9 +1306,9 @@
       <c r="I14" s="10"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="38"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
+      <c r="A15" s="57"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="61"/>
       <c r="D15" s="6">
         <v>1.5</v>
       </c>
@@ -1328,9 +1328,9 @@
       <c r="I15" s="10"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="38"/>
-      <c r="B16" s="44"/>
-      <c r="C16" s="44"/>
+      <c r="A16" s="57"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
       <c r="D16" s="6">
         <v>1.75</v>
       </c>
@@ -1350,9 +1350,9 @@
       <c r="I16" s="10"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="38"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="44"/>
+      <c r="A17" s="57"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="61"/>
       <c r="D17" s="6">
         <v>2</v>
       </c>
@@ -1372,11 +1372,11 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="38"/>
-      <c r="B18" s="34">
+      <c r="A18" s="57"/>
+      <c r="B18" s="53">
         <v>1</v>
       </c>
-      <c r="C18" s="44"/>
+      <c r="C18" s="61"/>
       <c r="D18" s="6">
         <v>1.25</v>
       </c>
@@ -1396,9 +1396,9 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="38"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="44"/>
+      <c r="A19" s="57"/>
+      <c r="B19" s="54"/>
+      <c r="C19" s="61"/>
       <c r="D19" s="6">
         <v>1.5</v>
       </c>
@@ -1418,9 +1418,9 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="38"/>
-      <c r="B20" s="35"/>
-      <c r="C20" s="44"/>
+      <c r="A20" s="57"/>
+      <c r="B20" s="54"/>
+      <c r="C20" s="61"/>
       <c r="D20" s="6">
         <v>1.75</v>
       </c>
@@ -1440,9 +1440,9 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="38"/>
-      <c r="B21" s="36"/>
-      <c r="C21" s="44"/>
+      <c r="A21" s="57"/>
+      <c r="B21" s="55"/>
+      <c r="C21" s="61"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1462,11 +1462,11 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="38"/>
-      <c r="B22" s="44">
+      <c r="A22" s="57"/>
+      <c r="B22" s="61">
         <v>0.75</v>
       </c>
-      <c r="C22" s="44"/>
+      <c r="C22" s="61"/>
       <c r="D22" s="6">
         <v>1.25</v>
       </c>
@@ -1486,9 +1486,9 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="38"/>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
+      <c r="A23" s="57"/>
+      <c r="B23" s="61"/>
+      <c r="C23" s="61"/>
       <c r="D23" s="6">
         <v>1.5</v>
       </c>
@@ -1507,9 +1507,9 @@
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="38"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
+      <c r="A24" s="57"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="61"/>
       <c r="D24" s="6">
         <v>1.75</v>
       </c>
@@ -1529,9 +1529,9 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="38"/>
-      <c r="B25" s="44"/>
-      <c r="C25" s="44"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="61"/>
       <c r="D25" s="6">
         <v>2</v>
       </c>
@@ -1551,11 +1551,11 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="38"/>
-      <c r="B26" s="44">
+      <c r="A26" s="57"/>
+      <c r="B26" s="61">
         <v>0.5</v>
       </c>
-      <c r="C26" s="44"/>
+      <c r="C26" s="61"/>
       <c r="D26" s="6">
         <v>1.25</v>
       </c>
@@ -1575,9 +1575,9 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="38"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
+      <c r="A27" s="57"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="61"/>
       <c r="D27" s="6">
         <v>1.5</v>
       </c>
@@ -1597,9 +1597,9 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="38"/>
-      <c r="B28" s="44"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="57"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="61"/>
       <c r="D28" s="6">
         <v>1.75</v>
       </c>
@@ -1619,9 +1619,9 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="38"/>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="57"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="61"/>
       <c r="D29" s="6">
         <v>2</v>
       </c>
@@ -1641,11 +1641,11 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="38"/>
-      <c r="B30" s="44">
+      <c r="A30" s="57"/>
+      <c r="B30" s="61">
         <v>0.25</v>
       </c>
-      <c r="C30" s="44"/>
+      <c r="C30" s="61"/>
       <c r="D30" s="6">
         <v>1.25</v>
       </c>
@@ -1665,9 +1665,9 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="38"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="44"/>
+      <c r="A31" s="57"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="61"/>
       <c r="D31" s="6">
         <v>1.5</v>
       </c>
@@ -1687,9 +1687,9 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="38"/>
-      <c r="B32" s="44"/>
-      <c r="C32" s="44"/>
+      <c r="A32" s="57"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="61"/>
       <c r="D32" s="6">
         <v>1.75</v>
       </c>
@@ -1709,9 +1709,9 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="39"/>
-      <c r="B33" s="45"/>
-      <c r="C33" s="45"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
       <c r="D33" s="8">
         <v>2</v>
       </c>
@@ -1731,13 +1731,13 @@
       <c r="I33" s="10"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="40" t="s">
+      <c r="A34" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="B34" s="46">
+      <c r="B34" s="63">
         <v>0.1</v>
       </c>
-      <c r="C34" s="46">
+      <c r="C34" s="63">
         <v>1</v>
       </c>
       <c r="D34" s="4">
@@ -1759,9 +1759,9 @@
       <c r="I34" s="10"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="41"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
+      <c r="A35" s="39"/>
+      <c r="B35" s="61"/>
+      <c r="C35" s="61"/>
       <c r="D35" s="6">
         <v>1.5</v>
       </c>
@@ -1781,9 +1781,9 @@
       <c r="I35" s="10"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="41"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
+      <c r="A36" s="39"/>
+      <c r="B36" s="61"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="6">
         <v>1.75</v>
       </c>
@@ -1803,9 +1803,9 @@
       <c r="I36" s="10"/>
     </row>
     <row r="37" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="42"/>
-      <c r="B37" s="45"/>
-      <c r="C37" s="45"/>
+      <c r="A37" s="38"/>
+      <c r="B37" s="62"/>
+      <c r="C37" s="62"/>
       <c r="D37" s="8">
         <v>2</v>
       </c>
@@ -1825,14 +1825,14 @@
       <c r="I37" s="10"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="47" t="s">
+      <c r="A38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C38" s="55"/>
-      <c r="D38" s="56"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="45"/>
       <c r="E38" s="4">
         <v>42.087400000000002</v>
       </c>
@@ -1849,12 +1849,12 @@
       <c r="I38" s="10"/>
     </row>
     <row r="39" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="42"/>
-      <c r="B39" s="48" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C39" s="49"/>
-      <c r="D39" s="50"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="42"/>
       <c r="E39" s="13">
         <v>42.128999999999998</v>
       </c>
@@ -1871,13 +1871,13 @@
       <c r="I39" s="10"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="B40" s="61" t="s">
+      <c r="B40" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C40" s="62"/>
+      <c r="C40" s="51"/>
       <c r="D40" s="4" t="s">
         <v>15</v>
       </c>
@@ -1899,9 +1899,9 @@
       <c r="I40" s="10"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="41"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="63"/>
+      <c r="A41" s="39"/>
+      <c r="B41" s="43"/>
+      <c r="C41" s="52"/>
       <c r="D41" s="6" t="s">
         <v>14</v>
       </c>
@@ -1923,11 +1923,11 @@
       <c r="I41" s="10"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="41"/>
-      <c r="B42" s="57" t="s">
+      <c r="A42" s="39"/>
+      <c r="B42" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="C42" s="58"/>
+      <c r="C42" s="47"/>
       <c r="D42" s="6" t="s">
         <v>15</v>
       </c>
@@ -1949,9 +1949,9 @@
       <c r="I42" s="10"/>
     </row>
     <row r="43" spans="1:9" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="42"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="60"/>
+      <c r="A43" s="38"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
       <c r="D43" s="8" t="s">
         <v>14</v>
       </c>
@@ -1973,14 +1973,14 @@
       <c r="I43" s="10"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="B44" s="51" t="s">
+      <c r="B44" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="C44" s="52"/>
-      <c r="D44" s="53"/>
+      <c r="C44" s="35"/>
+      <c r="D44" s="36"/>
       <c r="E44" s="4">
         <v>42.231000000000002</v>
       </c>
@@ -1997,12 +1997,12 @@
       <c r="I44" s="10"/>
     </row>
     <row r="45" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A45" s="42"/>
-      <c r="B45" s="48" t="s">
+      <c r="A45" s="38"/>
+      <c r="B45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="49"/>
-      <c r="D45" s="50"/>
+      <c r="C45" s="41"/>
+      <c r="D45" s="42"/>
       <c r="E45" s="13">
         <v>42.606000000000002</v>
       </c>
@@ -2019,12 +2019,12 @@
       <c r="I45" s="10"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="43" t="s">
+      <c r="A46" s="60" t="s">
         <v>1</v>
       </c>
-      <c r="B46" s="43"/>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
+      <c r="B46" s="60"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="60"/>
       <c r="E46" s="5">
         <v>42.67</v>
       </c>
@@ -2051,13 +2051,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B42:C43"/>
-    <mergeCell ref="B40:C41"/>
     <mergeCell ref="B18:B21"/>
     <mergeCell ref="A2:A33"/>
     <mergeCell ref="A34:A37"/>
@@ -2074,6 +2067,13 @@
     <mergeCell ref="C34:C37"/>
     <mergeCell ref="A44:A45"/>
     <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A38:A39"/>
+    <mergeCell ref="A40:A43"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B42:C43"/>
+    <mergeCell ref="B40:C41"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -2085,7 +2085,7 @@
   <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2488,7 +2488,7 @@
       <c r="I17" s="10"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -2514,7 +2514,7 @@
       <c r="I18" s="10"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -2536,7 +2536,7 @@
       <c r="I19" s="10"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -2558,7 +2558,7 @@
       <c r="I20" s="10"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -2580,7 +2580,7 @@
       <c r="I21" s="10"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>5</v>
       </c>
@@ -2606,7 +2606,7 @@
       <c r="I22" s="10"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -2627,7 +2627,7 @@
       <c r="H23" s="28"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -2649,7 +2649,7 @@
       <c r="I24" s="10"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -2671,7 +2671,7 @@
       <c r="I25" s="10"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>6</v>
       </c>
@@ -2695,7 +2695,7 @@
       <c r="I26" s="10"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -2717,7 +2717,7 @@
       <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -2739,7 +2739,7 @@
       <c r="I28" s="10"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -2761,7 +2761,7 @@
       <c r="I29" s="10"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>7</v>
       </c>
@@ -2785,7 +2785,7 @@
       <c r="I30" s="10"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -2807,7 +2807,7 @@
       <c r="I31" s="10"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -2829,7 +2829,7 @@
       <c r="I32" s="10"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3024,7 +3024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B44CA5E-D6A9-491D-9F24-D323A0E66CBD}">
   <dimension ref="A1:I33"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
@@ -3397,7 +3397,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="65">
@@ -3421,7 +3421,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="65"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -3441,7 +3441,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="65"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -3461,7 +3461,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="66"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -3481,7 +3481,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="67">
         <v>0.4</v>
       </c>
@@ -3503,7 +3503,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="65"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -3523,7 +3523,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="65"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -3543,7 +3543,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="66"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -3563,7 +3563,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="67">
         <v>0.6</v>
       </c>
@@ -3585,7 +3585,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="65"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -3608,7 +3608,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="65"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -3628,7 +3628,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="66"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -3648,7 +3648,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="67">
         <v>0.8</v>
       </c>
@@ -3670,7 +3670,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="65"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -3690,7 +3690,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="65"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -3710,7 +3710,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="66"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -3731,16 +3731,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -4123,7 +4123,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="34" t="s">
+      <c r="A18" s="53" t="s">
         <v>21</v>
       </c>
       <c r="B18" s="68">
@@ -4147,7 +4147,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="35"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="68"/>
       <c r="C19" s="23">
         <v>1.5</v>
@@ -4167,7 +4167,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="35"/>
+      <c r="A20" s="54"/>
       <c r="B20" s="68"/>
       <c r="C20" s="23">
         <v>1.75</v>
@@ -4187,7 +4187,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="35"/>
+      <c r="A21" s="54"/>
       <c r="B21" s="68"/>
       <c r="C21" s="23">
         <v>2</v>
@@ -4207,7 +4207,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="35"/>
+      <c r="A22" s="54"/>
       <c r="B22" s="68">
         <v>1</v>
       </c>
@@ -4229,7 +4229,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="35"/>
+      <c r="A23" s="54"/>
       <c r="B23" s="68"/>
       <c r="C23" s="23">
         <v>1.5</v>
@@ -4249,7 +4249,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="35"/>
+      <c r="A24" s="54"/>
       <c r="B24" s="68"/>
       <c r="C24" s="23">
         <v>1.75</v>
@@ -4269,7 +4269,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="35"/>
+      <c r="A25" s="54"/>
       <c r="B25" s="68"/>
       <c r="C25" s="23">
         <v>2</v>
@@ -4289,7 +4289,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="35"/>
+      <c r="A26" s="54"/>
       <c r="B26" s="68">
         <v>2</v>
       </c>
@@ -4311,7 +4311,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="35"/>
+      <c r="A27" s="54"/>
       <c r="B27" s="68"/>
       <c r="C27" s="23">
         <v>1.5</v>
@@ -4331,7 +4331,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="35"/>
+      <c r="A28" s="54"/>
       <c r="B28" s="68"/>
       <c r="C28" s="23">
         <v>1.75</v>
@@ -4351,7 +4351,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="35"/>
+      <c r="A29" s="54"/>
       <c r="B29" s="68"/>
       <c r="C29" s="23">
         <v>2</v>
@@ -4371,7 +4371,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="35"/>
+      <c r="A30" s="54"/>
       <c r="B30" s="68">
         <v>3</v>
       </c>
@@ -4393,7 +4393,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="35"/>
+      <c r="A31" s="54"/>
       <c r="B31" s="68"/>
       <c r="C31" s="23">
         <v>1.5</v>
@@ -4413,7 +4413,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="35"/>
+      <c r="A32" s="54"/>
       <c r="B32" s="68"/>
       <c r="C32" s="23">
         <v>1.75</v>
@@ -4433,7 +4433,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" s="36"/>
+      <c r="A33" s="55"/>
       <c r="B33" s="68"/>
       <c r="C33" s="23">
         <v>2</v>
@@ -4459,16 +4459,16 @@
     <row r="47" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A18:A33"/>
+    <mergeCell ref="B18:B21"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B33"/>
     <mergeCell ref="A2:A17"/>
     <mergeCell ref="B2:B5"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B13"/>
     <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A18:A33"/>
-    <mergeCell ref="B18:B21"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="B26:B29"/>
-    <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -5174,7 +5174,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71968B89-5396-4DBB-9374-8D1D5CD3665B}">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
@@ -6208,12 +6208,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -6446,17 +6445,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
+    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -6481,18 +6490,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E9D27D8-044D-44EB-88DB-642AFEB3F345}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E308881-5124-4B0A-82DE-B3088F1EAF79}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="1a03cb65-d35a-4d70-82d7-cdf046b799c1"/>
-    <ds:schemaRef ds:uri="66f5e48b-5e03-411e-a0b5-f2048ddf7ea4"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>